<commit_message>
updating minutes and gantt chart
</commit_message>
<xml_diff>
--- a/0b_forms/gantt_chart.xlsx
+++ b/0b_forms/gantt_chart.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="460" windowWidth="33600" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="GanttChart" sheetId="9" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="prevWBS" localSheetId="0">GanttChart!$A1048576</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">GanttChart!$A$1:$BN$65</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">GanttChartPro!$A$1:$C$47</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">GanttChart!$4:$7</definedName>
     <definedName name="valuevx">42.314159</definedName>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="187">
   <si>
     <t>WBS</t>
   </si>
@@ -1291,9 +1291,6 @@
     <t>Evaluation plan</t>
   </si>
   <si>
-    <t>Project management</t>
-  </si>
-  <si>
     <t>Conclusion</t>
   </si>
   <si>
@@ -1316,6 +1313,12 @@
   </si>
   <si>
     <t>User stories and acceptane stories</t>
+  </si>
+  <si>
+    <t>Project Management</t>
+  </si>
+  <si>
+    <t>Systems Requirements Specification</t>
   </si>
 </sst>
 </file>
@@ -2645,13 +2648,6 @@
     <xf numFmtId="0" fontId="40" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2661,10 +2657,6 @@
     <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="43" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="167" fontId="43" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2673,6 +2665,17 @@
     </xf>
     <xf numFmtId="167" fontId="43" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="43" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2724,7 +2727,59 @@
     <cellStyle name="Total" xfId="42" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="43" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="66">
+  <dxfs count="75">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -3415,6 +3470,32 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -3503,7 +3584,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="8"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$4" horiz="1" max="100" min="1" page="0" val="6"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3526,7 +3607,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3590,7 +3671,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3640,7 +3721,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3724,7 +3805,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3779,7 +3860,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3834,7 +3915,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4159,11 +4240,11 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN71"/>
+  <dimension ref="A1:BN72"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B63" sqref="B63"/>
+      <pane ySplit="7" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4191,27 +4272,27 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="129"/>
-      <c r="K1" s="162"/>
-      <c r="L1" s="162"/>
-      <c r="M1" s="162"/>
-      <c r="N1" s="162"/>
-      <c r="O1" s="162"/>
-      <c r="P1" s="162"/>
-      <c r="Q1" s="162"/>
-      <c r="R1" s="162"/>
-      <c r="S1" s="162"/>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
+      <c r="K1" s="168"/>
+      <c r="L1" s="168"/>
+      <c r="M1" s="168"/>
+      <c r="N1" s="168"/>
+      <c r="O1" s="168"/>
+      <c r="P1" s="168"/>
+      <c r="Q1" s="168"/>
+      <c r="R1" s="168"/>
+      <c r="S1" s="168"/>
+      <c r="T1" s="168"/>
+      <c r="U1" s="168"/>
+      <c r="V1" s="168"/>
+      <c r="W1" s="168"/>
+      <c r="X1" s="168"/>
+      <c r="Y1" s="168"/>
+      <c r="Z1" s="168"/>
+      <c r="AA1" s="168"/>
+      <c r="AB1" s="168"/>
+      <c r="AC1" s="168"/>
+      <c r="AD1" s="168"/>
+      <c r="AE1" s="168"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="52" t="s">
@@ -4256,196 +4337,196 @@
       <c r="B4" s="113" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="167">
+      <c r="C4" s="170">
         <v>43374</v>
       </c>
-      <c r="D4" s="167"/>
-      <c r="E4" s="167"/>
+      <c r="D4" s="170"/>
+      <c r="E4" s="170"/>
       <c r="F4" s="110"/>
       <c r="G4" s="113" t="s">
         <v>73</v>
       </c>
       <c r="H4" s="126">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I4" s="111"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="164" t="str">
+      <c r="K4" s="162" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 6</v>
+      </c>
+      <c r="L4" s="163"/>
+      <c r="M4" s="163"/>
+      <c r="N4" s="163"/>
+      <c r="O4" s="163"/>
+      <c r="P4" s="163"/>
+      <c r="Q4" s="164"/>
+      <c r="R4" s="162" t="str">
+        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+        <v>Week 7</v>
+      </c>
+      <c r="S4" s="163"/>
+      <c r="T4" s="163"/>
+      <c r="U4" s="163"/>
+      <c r="V4" s="163"/>
+      <c r="W4" s="163"/>
+      <c r="X4" s="164"/>
+      <c r="Y4" s="162" t="str">
+        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="L4" s="165"/>
-      <c r="M4" s="165"/>
-      <c r="N4" s="165"/>
-      <c r="O4" s="165"/>
-      <c r="P4" s="165"/>
-      <c r="Q4" s="166"/>
-      <c r="R4" s="164" t="str">
-        <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="Z4" s="163"/>
+      <c r="AA4" s="163"/>
+      <c r="AB4" s="163"/>
+      <c r="AC4" s="163"/>
+      <c r="AD4" s="163"/>
+      <c r="AE4" s="164"/>
+      <c r="AF4" s="162" t="str">
+        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="S4" s="165"/>
-      <c r="T4" s="165"/>
-      <c r="U4" s="165"/>
-      <c r="V4" s="165"/>
-      <c r="W4" s="165"/>
-      <c r="X4" s="166"/>
-      <c r="Y4" s="164" t="str">
-        <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AG4" s="163"/>
+      <c r="AH4" s="163"/>
+      <c r="AI4" s="163"/>
+      <c r="AJ4" s="163"/>
+      <c r="AK4" s="163"/>
+      <c r="AL4" s="164"/>
+      <c r="AM4" s="162" t="str">
+        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="Z4" s="165"/>
-      <c r="AA4" s="165"/>
-      <c r="AB4" s="165"/>
-      <c r="AC4" s="165"/>
-      <c r="AD4" s="165"/>
-      <c r="AE4" s="166"/>
-      <c r="AF4" s="164" t="str">
-        <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AN4" s="163"/>
+      <c r="AO4" s="163"/>
+      <c r="AP4" s="163"/>
+      <c r="AQ4" s="163"/>
+      <c r="AR4" s="163"/>
+      <c r="AS4" s="164"/>
+      <c r="AT4" s="162" t="str">
+        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="AG4" s="165"/>
-      <c r="AH4" s="165"/>
-      <c r="AI4" s="165"/>
-      <c r="AJ4" s="165"/>
-      <c r="AK4" s="165"/>
-      <c r="AL4" s="166"/>
-      <c r="AM4" s="164" t="str">
-        <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="AU4" s="163"/>
+      <c r="AV4" s="163"/>
+      <c r="AW4" s="163"/>
+      <c r="AX4" s="163"/>
+      <c r="AY4" s="163"/>
+      <c r="AZ4" s="164"/>
+      <c r="BA4" s="162" t="str">
+        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 12</v>
       </c>
-      <c r="AN4" s="165"/>
-      <c r="AO4" s="165"/>
-      <c r="AP4" s="165"/>
-      <c r="AQ4" s="165"/>
-      <c r="AR4" s="165"/>
-      <c r="AS4" s="166"/>
-      <c r="AT4" s="164" t="str">
-        <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
+      <c r="BB4" s="163"/>
+      <c r="BC4" s="163"/>
+      <c r="BD4" s="163"/>
+      <c r="BE4" s="163"/>
+      <c r="BF4" s="163"/>
+      <c r="BG4" s="164"/>
+      <c r="BH4" s="162" t="str">
+        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 13</v>
       </c>
-      <c r="AU4" s="165"/>
-      <c r="AV4" s="165"/>
-      <c r="AW4" s="165"/>
-      <c r="AX4" s="165"/>
-      <c r="AY4" s="165"/>
-      <c r="AZ4" s="166"/>
-      <c r="BA4" s="164" t="str">
-        <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 14</v>
-      </c>
-      <c r="BB4" s="165"/>
-      <c r="BC4" s="165"/>
-      <c r="BD4" s="165"/>
-      <c r="BE4" s="165"/>
-      <c r="BF4" s="165"/>
-      <c r="BG4" s="166"/>
-      <c r="BH4" s="164" t="str">
-        <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
-        <v>Week 15</v>
-      </c>
-      <c r="BI4" s="165"/>
-      <c r="BJ4" s="165"/>
-      <c r="BK4" s="165"/>
-      <c r="BL4" s="165"/>
-      <c r="BM4" s="165"/>
-      <c r="BN4" s="166"/>
+      <c r="BI4" s="163"/>
+      <c r="BJ4" s="163"/>
+      <c r="BK4" s="163"/>
+      <c r="BL4" s="163"/>
+      <c r="BM4" s="163"/>
+      <c r="BN4" s="164"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="109"/>
       <c r="B5" s="113" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="163">
+      <c r="C5" s="169">
         <v>43612</v>
       </c>
-      <c r="D5" s="163"/>
-      <c r="E5" s="163"/>
+      <c r="D5" s="169"/>
+      <c r="E5" s="169"/>
       <c r="F5" s="112"/>
       <c r="G5" s="112"/>
       <c r="H5" s="112"/>
       <c r="I5" s="112"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="168">
+      <c r="K5" s="165">
         <f>K6</f>
+        <v>43409</v>
+      </c>
+      <c r="L5" s="166"/>
+      <c r="M5" s="166"/>
+      <c r="N5" s="166"/>
+      <c r="O5" s="166"/>
+      <c r="P5" s="166"/>
+      <c r="Q5" s="167"/>
+      <c r="R5" s="165">
+        <f>R6</f>
+        <v>43416</v>
+      </c>
+      <c r="S5" s="166"/>
+      <c r="T5" s="166"/>
+      <c r="U5" s="166"/>
+      <c r="V5" s="166"/>
+      <c r="W5" s="166"/>
+      <c r="X5" s="167"/>
+      <c r="Y5" s="165">
+        <f>Y6</f>
         <v>43423</v>
       </c>
-      <c r="L5" s="169"/>
-      <c r="M5" s="169"/>
-      <c r="N5" s="169"/>
-      <c r="O5" s="169"/>
-      <c r="P5" s="169"/>
-      <c r="Q5" s="170"/>
-      <c r="R5" s="168">
-        <f>R6</f>
+      <c r="Z5" s="166"/>
+      <c r="AA5" s="166"/>
+      <c r="AB5" s="166"/>
+      <c r="AC5" s="166"/>
+      <c r="AD5" s="166"/>
+      <c r="AE5" s="167"/>
+      <c r="AF5" s="165">
+        <f>AF6</f>
         <v>43430</v>
       </c>
-      <c r="S5" s="169"/>
-      <c r="T5" s="169"/>
-      <c r="U5" s="169"/>
-      <c r="V5" s="169"/>
-      <c r="W5" s="169"/>
-      <c r="X5" s="170"/>
-      <c r="Y5" s="168">
-        <f>Y6</f>
+      <c r="AG5" s="166"/>
+      <c r="AH5" s="166"/>
+      <c r="AI5" s="166"/>
+      <c r="AJ5" s="166"/>
+      <c r="AK5" s="166"/>
+      <c r="AL5" s="167"/>
+      <c r="AM5" s="165">
+        <f>AM6</f>
         <v>43437</v>
       </c>
-      <c r="Z5" s="169"/>
-      <c r="AA5" s="169"/>
-      <c r="AB5" s="169"/>
-      <c r="AC5" s="169"/>
-      <c r="AD5" s="169"/>
-      <c r="AE5" s="170"/>
-      <c r="AF5" s="168">
-        <f>AF6</f>
+      <c r="AN5" s="166"/>
+      <c r="AO5" s="166"/>
+      <c r="AP5" s="166"/>
+      <c r="AQ5" s="166"/>
+      <c r="AR5" s="166"/>
+      <c r="AS5" s="167"/>
+      <c r="AT5" s="165">
+        <f>AT6</f>
         <v>43444</v>
       </c>
-      <c r="AG5" s="169"/>
-      <c r="AH5" s="169"/>
-      <c r="AI5" s="169"/>
-      <c r="AJ5" s="169"/>
-      <c r="AK5" s="169"/>
-      <c r="AL5" s="170"/>
-      <c r="AM5" s="168">
-        <f>AM6</f>
+      <c r="AU5" s="166"/>
+      <c r="AV5" s="166"/>
+      <c r="AW5" s="166"/>
+      <c r="AX5" s="166"/>
+      <c r="AY5" s="166"/>
+      <c r="AZ5" s="167"/>
+      <c r="BA5" s="165">
+        <f>BA6</f>
         <v>43451</v>
       </c>
-      <c r="AN5" s="169"/>
-      <c r="AO5" s="169"/>
-      <c r="AP5" s="169"/>
-      <c r="AQ5" s="169"/>
-      <c r="AR5" s="169"/>
-      <c r="AS5" s="170"/>
-      <c r="AT5" s="168">
-        <f>AT6</f>
+      <c r="BB5" s="166"/>
+      <c r="BC5" s="166"/>
+      <c r="BD5" s="166"/>
+      <c r="BE5" s="166"/>
+      <c r="BF5" s="166"/>
+      <c r="BG5" s="167"/>
+      <c r="BH5" s="165">
+        <f>BH6</f>
         <v>43458</v>
       </c>
-      <c r="AU5" s="169"/>
-      <c r="AV5" s="169"/>
-      <c r="AW5" s="169"/>
-      <c r="AX5" s="169"/>
-      <c r="AY5" s="169"/>
-      <c r="AZ5" s="170"/>
-      <c r="BA5" s="168">
-        <f>BA6</f>
-        <v>43465</v>
-      </c>
-      <c r="BB5" s="169"/>
-      <c r="BC5" s="169"/>
-      <c r="BD5" s="169"/>
-      <c r="BE5" s="169"/>
-      <c r="BF5" s="169"/>
-      <c r="BG5" s="170"/>
-      <c r="BH5" s="168">
-        <f>BH6</f>
-        <v>43472</v>
-      </c>
-      <c r="BI5" s="169"/>
-      <c r="BJ5" s="169"/>
-      <c r="BK5" s="169"/>
-      <c r="BL5" s="169"/>
-      <c r="BM5" s="169"/>
-      <c r="BN5" s="170"/>
+      <c r="BI5" s="166"/>
+      <c r="BJ5" s="166"/>
+      <c r="BK5" s="166"/>
+      <c r="BL5" s="166"/>
+      <c r="BM5" s="166"/>
+      <c r="BN5" s="167"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A6" s="49"/>
@@ -4460,227 +4541,227 @@
       <c r="J6" s="50"/>
       <c r="K6" s="92">
         <f>C4-WEEKDAY(C4,1)+2+7*(H4-1)</f>
-        <v>43423</v>
+        <v>43409</v>
       </c>
       <c r="L6" s="83">
         <f t="shared" ref="L6:AQ6" si="0">K6+1</f>
-        <v>43424</v>
+        <v>43410</v>
       </c>
       <c r="M6" s="83">
         <f t="shared" si="0"/>
-        <v>43425</v>
+        <v>43411</v>
       </c>
       <c r="N6" s="83">
         <f t="shared" si="0"/>
-        <v>43426</v>
+        <v>43412</v>
       </c>
       <c r="O6" s="83">
         <f t="shared" si="0"/>
-        <v>43427</v>
+        <v>43413</v>
       </c>
       <c r="P6" s="83">
         <f t="shared" si="0"/>
-        <v>43428</v>
+        <v>43414</v>
       </c>
       <c r="Q6" s="93">
         <f t="shared" si="0"/>
-        <v>43429</v>
+        <v>43415</v>
       </c>
       <c r="R6" s="92">
         <f t="shared" si="0"/>
-        <v>43430</v>
+        <v>43416</v>
       </c>
       <c r="S6" s="83">
         <f t="shared" si="0"/>
-        <v>43431</v>
+        <v>43417</v>
       </c>
       <c r="T6" s="83">
         <f t="shared" si="0"/>
-        <v>43432</v>
+        <v>43418</v>
       </c>
       <c r="U6" s="83">
         <f t="shared" si="0"/>
-        <v>43433</v>
+        <v>43419</v>
       </c>
       <c r="V6" s="83">
         <f t="shared" si="0"/>
-        <v>43434</v>
+        <v>43420</v>
       </c>
       <c r="W6" s="83">
         <f t="shared" si="0"/>
-        <v>43435</v>
+        <v>43421</v>
       </c>
       <c r="X6" s="93">
         <f t="shared" si="0"/>
-        <v>43436</v>
+        <v>43422</v>
       </c>
       <c r="Y6" s="92">
         <f t="shared" si="0"/>
-        <v>43437</v>
+        <v>43423</v>
       </c>
       <c r="Z6" s="83">
         <f t="shared" si="0"/>
-        <v>43438</v>
+        <v>43424</v>
       </c>
       <c r="AA6" s="83">
         <f t="shared" si="0"/>
-        <v>43439</v>
+        <v>43425</v>
       </c>
       <c r="AB6" s="83">
         <f t="shared" si="0"/>
-        <v>43440</v>
+        <v>43426</v>
       </c>
       <c r="AC6" s="83">
         <f t="shared" si="0"/>
-        <v>43441</v>
+        <v>43427</v>
       </c>
       <c r="AD6" s="83">
         <f t="shared" si="0"/>
-        <v>43442</v>
+        <v>43428</v>
       </c>
       <c r="AE6" s="93">
         <f t="shared" si="0"/>
-        <v>43443</v>
+        <v>43429</v>
       </c>
       <c r="AF6" s="92">
         <f t="shared" si="0"/>
-        <v>43444</v>
+        <v>43430</v>
       </c>
       <c r="AG6" s="83">
         <f t="shared" si="0"/>
-        <v>43445</v>
+        <v>43431</v>
       </c>
       <c r="AH6" s="83">
         <f t="shared" si="0"/>
-        <v>43446</v>
+        <v>43432</v>
       </c>
       <c r="AI6" s="83">
         <f t="shared" si="0"/>
-        <v>43447</v>
+        <v>43433</v>
       </c>
       <c r="AJ6" s="83">
         <f t="shared" si="0"/>
-        <v>43448</v>
+        <v>43434</v>
       </c>
       <c r="AK6" s="83">
         <f t="shared" si="0"/>
-        <v>43449</v>
+        <v>43435</v>
       </c>
       <c r="AL6" s="93">
         <f t="shared" si="0"/>
-        <v>43450</v>
+        <v>43436</v>
       </c>
       <c r="AM6" s="92">
         <f t="shared" si="0"/>
-        <v>43451</v>
+        <v>43437</v>
       </c>
       <c r="AN6" s="83">
         <f t="shared" si="0"/>
-        <v>43452</v>
+        <v>43438</v>
       </c>
       <c r="AO6" s="83">
         <f t="shared" si="0"/>
-        <v>43453</v>
+        <v>43439</v>
       </c>
       <c r="AP6" s="83">
         <f t="shared" si="0"/>
-        <v>43454</v>
+        <v>43440</v>
       </c>
       <c r="AQ6" s="83">
         <f t="shared" si="0"/>
-        <v>43455</v>
+        <v>43441</v>
       </c>
       <c r="AR6" s="83">
         <f t="shared" ref="AR6:BN6" si="1">AQ6+1</f>
-        <v>43456</v>
+        <v>43442</v>
       </c>
       <c r="AS6" s="93">
         <f t="shared" si="1"/>
-        <v>43457</v>
+        <v>43443</v>
       </c>
       <c r="AT6" s="92">
         <f t="shared" si="1"/>
-        <v>43458</v>
+        <v>43444</v>
       </c>
       <c r="AU6" s="83">
         <f t="shared" si="1"/>
-        <v>43459</v>
+        <v>43445</v>
       </c>
       <c r="AV6" s="83">
         <f t="shared" si="1"/>
-        <v>43460</v>
+        <v>43446</v>
       </c>
       <c r="AW6" s="83">
         <f t="shared" si="1"/>
-        <v>43461</v>
+        <v>43447</v>
       </c>
       <c r="AX6" s="83">
         <f t="shared" si="1"/>
-        <v>43462</v>
+        <v>43448</v>
       </c>
       <c r="AY6" s="83">
         <f t="shared" si="1"/>
-        <v>43463</v>
+        <v>43449</v>
       </c>
       <c r="AZ6" s="93">
         <f t="shared" si="1"/>
-        <v>43464</v>
+        <v>43450</v>
       </c>
       <c r="BA6" s="92">
         <f t="shared" si="1"/>
-        <v>43465</v>
+        <v>43451</v>
       </c>
       <c r="BB6" s="83">
         <f t="shared" si="1"/>
-        <v>43466</v>
+        <v>43452</v>
       </c>
       <c r="BC6" s="83">
         <f t="shared" si="1"/>
-        <v>43467</v>
+        <v>43453</v>
       </c>
       <c r="BD6" s="83">
         <f t="shared" si="1"/>
-        <v>43468</v>
+        <v>43454</v>
       </c>
       <c r="BE6" s="83">
         <f t="shared" si="1"/>
-        <v>43469</v>
+        <v>43455</v>
       </c>
       <c r="BF6" s="83">
         <f t="shared" si="1"/>
-        <v>43470</v>
+        <v>43456</v>
       </c>
       <c r="BG6" s="93">
         <f t="shared" si="1"/>
-        <v>43471</v>
+        <v>43457</v>
       </c>
       <c r="BH6" s="92">
         <f t="shared" si="1"/>
-        <v>43472</v>
+        <v>43458</v>
       </c>
       <c r="BI6" s="83">
         <f t="shared" si="1"/>
-        <v>43473</v>
+        <v>43459</v>
       </c>
       <c r="BJ6" s="83">
         <f t="shared" si="1"/>
-        <v>43474</v>
+        <v>43460</v>
       </c>
       <c r="BK6" s="83">
         <f t="shared" si="1"/>
-        <v>43475</v>
+        <v>43461</v>
       </c>
       <c r="BL6" s="83">
         <f t="shared" si="1"/>
-        <v>43476</v>
+        <v>43462</v>
       </c>
       <c r="BM6" s="83">
         <f t="shared" si="1"/>
-        <v>43477</v>
+        <v>43463</v>
       </c>
       <c r="BN6" s="93">
         <f t="shared" si="1"/>
-        <v>43478</v>
+        <v>43464</v>
       </c>
     </row>
     <row r="7" spans="1:66" s="160" customFormat="1" ht="25" thickBot="1" x14ac:dyDescent="0.2">
@@ -4955,7 +5036,7 @@
       <c r="G8" s="89"/>
       <c r="H8" s="90"/>
       <c r="I8" s="91" t="str">
-        <f t="shared" ref="I8:I64" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
+        <f t="shared" ref="I8:I65" si="4">IF(OR(F8=0,E8=0)," - ",NETWORKDAYS(E8,F8))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J8" s="94"/>
@@ -6941,7 +7022,7 @@
         <v>4.8</v>
       </c>
       <c r="B32" s="81" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C32" s="81"/>
       <c r="D32" s="79"/>
@@ -7104,7 +7185,7 @@
         <v>5.1</v>
       </c>
       <c r="B34" s="81" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C34" s="81"/>
       <c r="D34" s="79"/>
@@ -7118,7 +7199,9 @@
       <c r="G34" s="62">
         <v>7</v>
       </c>
-      <c r="H34" s="63"/>
+      <c r="H34" s="63">
+        <v>1</v>
+      </c>
       <c r="I34" s="80">
         <f t="shared" si="17"/>
         <v>5</v>
@@ -7187,7 +7270,7 @@
         <v>5.2</v>
       </c>
       <c r="B35" s="81" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C35" s="81"/>
       <c r="D35" s="79"/>
@@ -7201,7 +7284,9 @@
       <c r="G35" s="62">
         <v>4</v>
       </c>
-      <c r="H35" s="63"/>
+      <c r="H35" s="63">
+        <v>1</v>
+      </c>
       <c r="I35" s="80">
         <f t="shared" ref="I35:I36" si="20">IF(OR(F35=0,E35=0)," - ",NETWORKDAYS(E35,F35))</f>
         <v>4</v>
@@ -7270,7 +7355,7 @@
         <v>5.3</v>
       </c>
       <c r="B36" s="81" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C36" s="81"/>
       <c r="D36" s="79"/>
@@ -7284,7 +7369,9 @@
       <c r="G36" s="62">
         <v>7</v>
       </c>
-      <c r="H36" s="63"/>
+      <c r="H36" s="63">
+        <v>0.5</v>
+      </c>
       <c r="I36" s="80">
         <f t="shared" si="20"/>
         <v>5</v>
@@ -7353,7 +7440,7 @@
         <v>5.4</v>
       </c>
       <c r="B37" s="81" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C37" s="81"/>
       <c r="D37" s="79"/>
@@ -7367,7 +7454,9 @@
       <c r="G37" s="62">
         <v>4</v>
       </c>
-      <c r="H37" s="63"/>
+      <c r="H37" s="63">
+        <v>0</v>
+      </c>
       <c r="I37" s="80">
         <f t="shared" ref="I37:I39" si="22">IF(OR(F37=0,E37=0)," - ",NETWORKDAYS(E37,F37))</f>
         <v>4</v>
@@ -7436,7 +7525,7 @@
         <v>5.5</v>
       </c>
       <c r="B38" s="81" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C38" s="81"/>
       <c r="D38" s="79"/>
@@ -7519,7 +7608,7 @@
         <v>5.6</v>
       </c>
       <c r="B39" s="81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C39" s="81"/>
       <c r="D39" s="79"/>
@@ -7533,7 +7622,9 @@
       <c r="G39" s="62">
         <v>9</v>
       </c>
-      <c r="H39" s="63"/>
+      <c r="H39" s="63">
+        <v>0.25</v>
+      </c>
       <c r="I39" s="80">
         <f t="shared" si="22"/>
         <v>7</v>
@@ -7831,7 +7922,7 @@
     </row>
     <row r="43" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A43" s="60" t="str">
-        <f t="shared" ref="A43:A53" si="27">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A43:A54" si="27">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>7.1</v>
       </c>
       <c r="B43" s="81" t="s">
@@ -7928,7 +8019,7 @@
         <v>43388</v>
       </c>
       <c r="F44" s="101">
-        <f t="shared" ref="F44:F61" si="28">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
+        <f t="shared" ref="F44:F62" si="28">IF(ISBLANK(E44)," - ",IF(G44=0,E44,E44+G44-1))</f>
         <v>43391</v>
       </c>
       <c r="G44" s="62">
@@ -7938,7 +8029,7 @@
         <v>1</v>
       </c>
       <c r="I44" s="80">
-        <f t="shared" ref="I44:I61" si="29">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
+        <f t="shared" ref="I44:I62" si="29">IF(OR(F44=0,E44=0)," - ",NETWORKDAYS(E44,F44))</f>
         <v>4</v>
       </c>
       <c r="J44" s="99"/>
@@ -8103,7 +8194,7 @@
         <v>7</v>
       </c>
       <c r="H46" s="63">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="I46" s="80">
         <f t="shared" si="29"/>
@@ -8188,7 +8279,7 @@
         <v>7</v>
       </c>
       <c r="H47" s="63">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="I47" s="80">
         <f t="shared" si="29"/>
@@ -8266,7 +8357,7 @@
         <v>43423</v>
       </c>
       <c r="F48" s="101">
-        <f t="shared" ref="F48:F53" si="30">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
+        <f t="shared" ref="F48:F52" si="30">IF(ISBLANK(E48)," - ",IF(G48=0,E48,E48+G48-1))</f>
         <v>43429</v>
       </c>
       <c r="G48" s="62">
@@ -8276,7 +8367,7 @@
         <v>0.75</v>
       </c>
       <c r="I48" s="80">
-        <f t="shared" ref="I48:I53" si="31">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
+        <f t="shared" ref="I48:I52" si="31">IF(OR(F48=0,E48=0)," - ",NETWORKDAYS(E48,F48))</f>
         <v>5</v>
       </c>
       <c r="J48" s="99"/>
@@ -8343,26 +8434,24 @@
         <v>7.7</v>
       </c>
       <c r="B49" s="81" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C49" s="81"/>
       <c r="D49" s="79"/>
       <c r="E49" s="100">
-        <v>43388</v>
+        <v>43437</v>
       </c>
       <c r="F49" s="101">
         <f>IF(ISBLANK(E49)," - ",IF(G49=0,E49,E49+G49-1))</f>
-        <v>43391</v>
+        <v>43442</v>
       </c>
       <c r="G49" s="62">
-        <v>4</v>
-      </c>
-      <c r="H49" s="63">
-        <v>0.95</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="H49" s="63"/>
       <c r="I49" s="80">
         <f>IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J49" s="99"/>
       <c r="K49" s="107"/>
@@ -8428,7 +8517,7 @@
         <v>7.8</v>
       </c>
       <c r="B50" s="81" t="s">
-        <v>175</v>
+        <v>186</v>
       </c>
       <c r="C50" s="81"/>
       <c r="D50" s="79"/>
@@ -8442,9 +8531,7 @@
       <c r="G50" s="62">
         <v>6</v>
       </c>
-      <c r="H50" s="63">
-        <v>0.05</v>
-      </c>
+      <c r="H50" s="63"/>
       <c r="I50" s="80">
         <f>IF(OR(F50=0,E50=0)," - ",NETWORKDAYS(E50,F50))</f>
         <v>5</v>
@@ -8513,24 +8600,26 @@
         <v>7.9</v>
       </c>
       <c r="B51" s="81" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C51" s="81"/>
       <c r="D51" s="79"/>
       <c r="E51" s="100">
-        <v>43437</v>
+        <v>43388</v>
       </c>
       <c r="F51" s="101">
         <f t="shared" si="30"/>
-        <v>43442</v>
+        <v>43391</v>
       </c>
       <c r="G51" s="62">
-        <v>6</v>
-      </c>
-      <c r="H51" s="63"/>
+        <v>4</v>
+      </c>
+      <c r="H51" s="63">
+        <v>1</v>
+      </c>
       <c r="I51" s="80">
         <f t="shared" si="31"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J51" s="99"/>
       <c r="K51" s="107"/>
@@ -8596,7 +8685,7 @@
         <v>7.10</v>
       </c>
       <c r="B52" s="81" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C52" s="81"/>
       <c r="D52" s="79"/>
@@ -8679,24 +8768,24 @@
         <v>7.11</v>
       </c>
       <c r="B53" s="81" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="C53" s="81"/>
       <c r="D53" s="79"/>
       <c r="E53" s="100">
-        <v>43443</v>
+        <v>43437</v>
       </c>
       <c r="F53" s="101">
-        <f t="shared" si="30"/>
-        <v>43445</v>
+        <f>IF(ISBLANK(E53)," - ",IF(G53=0,E53,E53+G53-1))</f>
+        <v>43442</v>
       </c>
       <c r="G53" s="62">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H53" s="63"/>
       <c r="I53" s="80">
-        <f t="shared" si="31"/>
-        <v>2</v>
+        <f>IF(OR(F53=0,E53=0)," - ",NETWORKDAYS(E53,F53))</f>
+        <v>5</v>
       </c>
       <c r="J53" s="99"/>
       <c r="K53" s="107"/>
@@ -8756,795 +8845,807 @@
       <c r="BM53" s="107"/>
       <c r="BN53" s="107"/>
     </row>
-    <row r="54" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A54" s="53" t="str">
+    <row r="54" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A54" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>7.12</v>
+      </c>
+      <c r="B54" s="81" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="81"/>
+      <c r="D54" s="79"/>
+      <c r="E54" s="100">
+        <v>43446</v>
+      </c>
+      <c r="F54" s="101">
+        <f>IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
+        <v>43446</v>
+      </c>
+      <c r="G54" s="62">
+        <v>1</v>
+      </c>
+      <c r="H54" s="63"/>
+      <c r="I54" s="80">
+        <f>IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
+        <v>1</v>
+      </c>
+      <c r="J54" s="99"/>
+      <c r="K54" s="107"/>
+      <c r="L54" s="107"/>
+      <c r="M54" s="107"/>
+      <c r="N54" s="107"/>
+      <c r="O54" s="107"/>
+      <c r="P54" s="107"/>
+      <c r="Q54" s="107"/>
+      <c r="R54" s="107"/>
+      <c r="S54" s="107"/>
+      <c r="T54" s="107"/>
+      <c r="U54" s="107"/>
+      <c r="V54" s="107"/>
+      <c r="W54" s="107"/>
+      <c r="X54" s="107"/>
+      <c r="Y54" s="107"/>
+      <c r="Z54" s="107"/>
+      <c r="AA54" s="107"/>
+      <c r="AB54" s="107"/>
+      <c r="AC54" s="107"/>
+      <c r="AD54" s="107"/>
+      <c r="AE54" s="107"/>
+      <c r="AF54" s="107"/>
+      <c r="AG54" s="107"/>
+      <c r="AH54" s="107"/>
+      <c r="AI54" s="107"/>
+      <c r="AJ54" s="107"/>
+      <c r="AK54" s="107"/>
+      <c r="AL54" s="107"/>
+      <c r="AM54" s="107"/>
+      <c r="AN54" s="107"/>
+      <c r="AO54" s="107"/>
+      <c r="AP54" s="107"/>
+      <c r="AQ54" s="107"/>
+      <c r="AR54" s="107"/>
+      <c r="AS54" s="107"/>
+      <c r="AT54" s="107"/>
+      <c r="AU54" s="107"/>
+      <c r="AV54" s="107"/>
+      <c r="AW54" s="107"/>
+      <c r="AX54" s="107"/>
+      <c r="AY54" s="107"/>
+      <c r="AZ54" s="107"/>
+      <c r="BA54" s="107"/>
+      <c r="BB54" s="107"/>
+      <c r="BC54" s="107"/>
+      <c r="BD54" s="107"/>
+      <c r="BE54" s="107"/>
+      <c r="BF54" s="107"/>
+      <c r="BG54" s="107"/>
+      <c r="BH54" s="107"/>
+      <c r="BI54" s="107"/>
+      <c r="BJ54" s="107"/>
+      <c r="BK54" s="107"/>
+      <c r="BL54" s="107"/>
+      <c r="BM54" s="107"/>
+      <c r="BN54" s="107"/>
+    </row>
+    <row r="55" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A55" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>8</v>
       </c>
-      <c r="B54" s="54" t="s">
+      <c r="B55" s="54" t="s">
         <v>152</v>
       </c>
-      <c r="D54" s="56"/>
-      <c r="E54" s="102"/>
-      <c r="F54" s="102" t="str">
-        <f>IF(ISBLANK(E54)," - ",IF(G54=0,E54,E54+G54-1))</f>
+      <c r="D55" s="56"/>
+      <c r="E55" s="102"/>
+      <c r="F55" s="102" t="str">
+        <f>IF(ISBLANK(E55)," - ",IF(G55=0,E55,E55+G55-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G54" s="57"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="59" t="str">
-        <f>IF(OR(F54=0,E54=0)," - ",NETWORKDAYS(E54,F54))</f>
+      <c r="G55" s="57"/>
+      <c r="H55" s="58"/>
+      <c r="I55" s="59" t="str">
+        <f>IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J54" s="96"/>
-      <c r="K54" s="108"/>
-      <c r="L54" s="108"/>
-      <c r="M54" s="108"/>
-      <c r="N54" s="108"/>
-      <c r="O54" s="108"/>
-      <c r="P54" s="108"/>
-      <c r="Q54" s="108"/>
-      <c r="R54" s="108"/>
-      <c r="S54" s="108"/>
-      <c r="T54" s="108"/>
-      <c r="U54" s="108"/>
-      <c r="V54" s="108"/>
-      <c r="W54" s="108"/>
-      <c r="X54" s="108"/>
-      <c r="Y54" s="108"/>
-      <c r="Z54" s="108"/>
-      <c r="AA54" s="108"/>
-      <c r="AB54" s="108"/>
-      <c r="AC54" s="108"/>
-      <c r="AD54" s="108"/>
-      <c r="AE54" s="108"/>
-      <c r="AF54" s="108"/>
-      <c r="AG54" s="108"/>
-      <c r="AH54" s="108"/>
-      <c r="AI54" s="108"/>
-      <c r="AJ54" s="108"/>
-      <c r="AK54" s="108"/>
-      <c r="AL54" s="108"/>
-      <c r="AM54" s="108"/>
-      <c r="AN54" s="108"/>
-      <c r="AO54" s="108"/>
-      <c r="AP54" s="108"/>
-      <c r="AQ54" s="108"/>
-      <c r="AR54" s="108"/>
-      <c r="AS54" s="108"/>
-      <c r="AT54" s="108"/>
-      <c r="AU54" s="108"/>
-      <c r="AV54" s="108"/>
-      <c r="AW54" s="108"/>
-      <c r="AX54" s="108"/>
-      <c r="AY54" s="108"/>
-      <c r="AZ54" s="108"/>
-      <c r="BA54" s="108"/>
-      <c r="BB54" s="108"/>
-      <c r="BC54" s="108"/>
-      <c r="BD54" s="108"/>
-      <c r="BE54" s="108"/>
-      <c r="BF54" s="108"/>
-      <c r="BG54" s="108"/>
-      <c r="BH54" s="108"/>
-      <c r="BI54" s="108"/>
-      <c r="BJ54" s="108"/>
-      <c r="BK54" s="108"/>
-      <c r="BL54" s="108"/>
-      <c r="BM54" s="108"/>
-      <c r="BN54" s="108"/>
-    </row>
-    <row r="55" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A55" s="60" t="str">
+      <c r="J55" s="96"/>
+      <c r="K55" s="108"/>
+      <c r="L55" s="108"/>
+      <c r="M55" s="108"/>
+      <c r="N55" s="108"/>
+      <c r="O55" s="108"/>
+      <c r="P55" s="108"/>
+      <c r="Q55" s="108"/>
+      <c r="R55" s="108"/>
+      <c r="S55" s="108"/>
+      <c r="T55" s="108"/>
+      <c r="U55" s="108"/>
+      <c r="V55" s="108"/>
+      <c r="W55" s="108"/>
+      <c r="X55" s="108"/>
+      <c r="Y55" s="108"/>
+      <c r="Z55" s="108"/>
+      <c r="AA55" s="108"/>
+      <c r="AB55" s="108"/>
+      <c r="AC55" s="108"/>
+      <c r="AD55" s="108"/>
+      <c r="AE55" s="108"/>
+      <c r="AF55" s="108"/>
+      <c r="AG55" s="108"/>
+      <c r="AH55" s="108"/>
+      <c r="AI55" s="108"/>
+      <c r="AJ55" s="108"/>
+      <c r="AK55" s="108"/>
+      <c r="AL55" s="108"/>
+      <c r="AM55" s="108"/>
+      <c r="AN55" s="108"/>
+      <c r="AO55" s="108"/>
+      <c r="AP55" s="108"/>
+      <c r="AQ55" s="108"/>
+      <c r="AR55" s="108"/>
+      <c r="AS55" s="108"/>
+      <c r="AT55" s="108"/>
+      <c r="AU55" s="108"/>
+      <c r="AV55" s="108"/>
+      <c r="AW55" s="108"/>
+      <c r="AX55" s="108"/>
+      <c r="AY55" s="108"/>
+      <c r="AZ55" s="108"/>
+      <c r="BA55" s="108"/>
+      <c r="BB55" s="108"/>
+      <c r="BC55" s="108"/>
+      <c r="BD55" s="108"/>
+      <c r="BE55" s="108"/>
+      <c r="BF55" s="108"/>
+      <c r="BG55" s="108"/>
+      <c r="BH55" s="108"/>
+      <c r="BI55" s="108"/>
+      <c r="BJ55" s="108"/>
+      <c r="BK55" s="108"/>
+      <c r="BL55" s="108"/>
+      <c r="BM55" s="108"/>
+      <c r="BN55" s="108"/>
+    </row>
+    <row r="56" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A56" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>8.1</v>
       </c>
-      <c r="B55" s="81"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="79"/>
-      <c r="E55" s="100"/>
-      <c r="F55" s="101" t="str">
-        <f>IF(ISBLANK(E55)," - ",IF(G55=0,E55,E55+G55-1))</f>
+      <c r="B56" s="81"/>
+      <c r="C56" s="81"/>
+      <c r="D56" s="79"/>
+      <c r="E56" s="100"/>
+      <c r="F56" s="101" t="str">
+        <f>IF(ISBLANK(E56)," - ",IF(G56=0,E56,E56+G56-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G55" s="62"/>
-      <c r="H55" s="63"/>
-      <c r="I55" s="80" t="str">
-        <f>IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
+      <c r="G56" s="62"/>
+      <c r="H56" s="63"/>
+      <c r="I56" s="80" t="str">
+        <f>IF(OR(F56=0,E56=0)," - ",NETWORKDAYS(E56,F56))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J55" s="99"/>
-      <c r="K55" s="107"/>
-      <c r="L55" s="107"/>
-      <c r="M55" s="107"/>
-      <c r="N55" s="107"/>
-      <c r="O55" s="107"/>
-      <c r="P55" s="107"/>
-      <c r="Q55" s="107"/>
-      <c r="R55" s="107"/>
-      <c r="S55" s="107"/>
-      <c r="T55" s="107"/>
-      <c r="U55" s="107"/>
-      <c r="V55" s="107"/>
-      <c r="W55" s="107"/>
-      <c r="X55" s="107"/>
-      <c r="Y55" s="107"/>
-      <c r="Z55" s="107"/>
-      <c r="AA55" s="107"/>
-      <c r="AB55" s="107"/>
-      <c r="AC55" s="107"/>
-      <c r="AD55" s="107"/>
-      <c r="AE55" s="107"/>
-      <c r="AF55" s="107"/>
-      <c r="AG55" s="107"/>
-      <c r="AH55" s="107"/>
-      <c r="AI55" s="107"/>
-      <c r="AJ55" s="107"/>
-      <c r="AK55" s="107"/>
-      <c r="AL55" s="107"/>
-      <c r="AM55" s="107"/>
-      <c r="AN55" s="107"/>
-      <c r="AO55" s="107"/>
-      <c r="AP55" s="107"/>
-      <c r="AQ55" s="107"/>
-      <c r="AR55" s="107"/>
-      <c r="AS55" s="107"/>
-      <c r="AT55" s="107"/>
-      <c r="AU55" s="107"/>
-      <c r="AV55" s="107"/>
-      <c r="AW55" s="107"/>
-      <c r="AX55" s="107"/>
-      <c r="AY55" s="107"/>
-      <c r="AZ55" s="107"/>
-      <c r="BA55" s="107"/>
-      <c r="BB55" s="107"/>
-      <c r="BC55" s="107"/>
-      <c r="BD55" s="107"/>
-      <c r="BE55" s="107"/>
-      <c r="BF55" s="107"/>
-      <c r="BG55" s="107"/>
-      <c r="BH55" s="107"/>
-      <c r="BI55" s="107"/>
-      <c r="BJ55" s="107"/>
-      <c r="BK55" s="107"/>
-      <c r="BL55" s="107"/>
-      <c r="BM55" s="107"/>
-      <c r="BN55" s="107"/>
-    </row>
-    <row r="56" spans="1:66" s="55" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A56" s="53" t="str">
+      <c r="J56" s="99"/>
+      <c r="K56" s="107"/>
+      <c r="L56" s="107"/>
+      <c r="M56" s="107"/>
+      <c r="N56" s="107"/>
+      <c r="O56" s="107"/>
+      <c r="P56" s="107"/>
+      <c r="Q56" s="107"/>
+      <c r="R56" s="107"/>
+      <c r="S56" s="107"/>
+      <c r="T56" s="107"/>
+      <c r="U56" s="107"/>
+      <c r="V56" s="107"/>
+      <c r="W56" s="107"/>
+      <c r="X56" s="107"/>
+      <c r="Y56" s="107"/>
+      <c r="Z56" s="107"/>
+      <c r="AA56" s="107"/>
+      <c r="AB56" s="107"/>
+      <c r="AC56" s="107"/>
+      <c r="AD56" s="107"/>
+      <c r="AE56" s="107"/>
+      <c r="AF56" s="107"/>
+      <c r="AG56" s="107"/>
+      <c r="AH56" s="107"/>
+      <c r="AI56" s="107"/>
+      <c r="AJ56" s="107"/>
+      <c r="AK56" s="107"/>
+      <c r="AL56" s="107"/>
+      <c r="AM56" s="107"/>
+      <c r="AN56" s="107"/>
+      <c r="AO56" s="107"/>
+      <c r="AP56" s="107"/>
+      <c r="AQ56" s="107"/>
+      <c r="AR56" s="107"/>
+      <c r="AS56" s="107"/>
+      <c r="AT56" s="107"/>
+      <c r="AU56" s="107"/>
+      <c r="AV56" s="107"/>
+      <c r="AW56" s="107"/>
+      <c r="AX56" s="107"/>
+      <c r="AY56" s="107"/>
+      <c r="AZ56" s="107"/>
+      <c r="BA56" s="107"/>
+      <c r="BB56" s="107"/>
+      <c r="BC56" s="107"/>
+      <c r="BD56" s="107"/>
+      <c r="BE56" s="107"/>
+      <c r="BF56" s="107"/>
+      <c r="BG56" s="107"/>
+      <c r="BH56" s="107"/>
+      <c r="BI56" s="107"/>
+      <c r="BJ56" s="107"/>
+      <c r="BK56" s="107"/>
+      <c r="BL56" s="107"/>
+      <c r="BM56" s="107"/>
+      <c r="BN56" s="107"/>
+    </row>
+    <row r="57" spans="1:66" s="55" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>9</v>
       </c>
-      <c r="B56" s="54" t="s">
+      <c r="B57" s="54" t="s">
         <v>154</v>
       </c>
-      <c r="D56" s="56"/>
-      <c r="E56" s="102"/>
-      <c r="F56" s="102" t="str">
-        <f t="shared" ref="F56:F57" si="32">IF(ISBLANK(E56)," - ",IF(G56=0,E56,E56+G56-1))</f>
+      <c r="D57" s="56"/>
+      <c r="E57" s="102"/>
+      <c r="F57" s="102" t="str">
+        <f t="shared" ref="F57:F58" si="32">IF(ISBLANK(E57)," - ",IF(G57=0,E57,E57+G57-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G56" s="57"/>
-      <c r="H56" s="58"/>
-      <c r="I56" s="59" t="str">
-        <f t="shared" ref="I56:I57" si="33">IF(OR(F56=0,E56=0)," - ",NETWORKDAYS(E56,F56))</f>
+      <c r="G57" s="57"/>
+      <c r="H57" s="58"/>
+      <c r="I57" s="59" t="str">
+        <f t="shared" ref="I57:I58" si="33">IF(OR(F57=0,E57=0)," - ",NETWORKDAYS(E57,F57))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J56" s="96"/>
-      <c r="K56" s="108"/>
-      <c r="L56" s="108"/>
-      <c r="M56" s="108"/>
-      <c r="N56" s="108"/>
-      <c r="O56" s="108"/>
-      <c r="P56" s="108"/>
-      <c r="Q56" s="108"/>
-      <c r="R56" s="108"/>
-      <c r="S56" s="108"/>
-      <c r="T56" s="108"/>
-      <c r="U56" s="108"/>
-      <c r="V56" s="108"/>
-      <c r="W56" s="108"/>
-      <c r="X56" s="108"/>
-      <c r="Y56" s="108"/>
-      <c r="Z56" s="108"/>
-      <c r="AA56" s="108"/>
-      <c r="AB56" s="108"/>
-      <c r="AC56" s="108"/>
-      <c r="AD56" s="108"/>
-      <c r="AE56" s="108"/>
-      <c r="AF56" s="108"/>
-      <c r="AG56" s="108"/>
-      <c r="AH56" s="108"/>
-      <c r="AI56" s="108"/>
-      <c r="AJ56" s="108"/>
-      <c r="AK56" s="108"/>
-      <c r="AL56" s="108"/>
-      <c r="AM56" s="108"/>
-      <c r="AN56" s="108"/>
-      <c r="AO56" s="108"/>
-      <c r="AP56" s="108"/>
-      <c r="AQ56" s="108"/>
-      <c r="AR56" s="108"/>
-      <c r="AS56" s="108"/>
-      <c r="AT56" s="108"/>
-      <c r="AU56" s="108"/>
-      <c r="AV56" s="108"/>
-      <c r="AW56" s="108"/>
-      <c r="AX56" s="108"/>
-      <c r="AY56" s="108"/>
-      <c r="AZ56" s="108"/>
-      <c r="BA56" s="108"/>
-      <c r="BB56" s="108"/>
-      <c r="BC56" s="108"/>
-      <c r="BD56" s="108"/>
-      <c r="BE56" s="108"/>
-      <c r="BF56" s="108"/>
-      <c r="BG56" s="108"/>
-      <c r="BH56" s="108"/>
-      <c r="BI56" s="108"/>
-      <c r="BJ56" s="108"/>
-      <c r="BK56" s="108"/>
-      <c r="BL56" s="108"/>
-      <c r="BM56" s="108"/>
-      <c r="BN56" s="108"/>
-    </row>
-    <row r="57" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A57" s="60" t="str">
+      <c r="J57" s="96"/>
+      <c r="K57" s="108"/>
+      <c r="L57" s="108"/>
+      <c r="M57" s="108"/>
+      <c r="N57" s="108"/>
+      <c r="O57" s="108"/>
+      <c r="P57" s="108"/>
+      <c r="Q57" s="108"/>
+      <c r="R57" s="108"/>
+      <c r="S57" s="108"/>
+      <c r="T57" s="108"/>
+      <c r="U57" s="108"/>
+      <c r="V57" s="108"/>
+      <c r="W57" s="108"/>
+      <c r="X57" s="108"/>
+      <c r="Y57" s="108"/>
+      <c r="Z57" s="108"/>
+      <c r="AA57" s="108"/>
+      <c r="AB57" s="108"/>
+      <c r="AC57" s="108"/>
+      <c r="AD57" s="108"/>
+      <c r="AE57" s="108"/>
+      <c r="AF57" s="108"/>
+      <c r="AG57" s="108"/>
+      <c r="AH57" s="108"/>
+      <c r="AI57" s="108"/>
+      <c r="AJ57" s="108"/>
+      <c r="AK57" s="108"/>
+      <c r="AL57" s="108"/>
+      <c r="AM57" s="108"/>
+      <c r="AN57" s="108"/>
+      <c r="AO57" s="108"/>
+      <c r="AP57" s="108"/>
+      <c r="AQ57" s="108"/>
+      <c r="AR57" s="108"/>
+      <c r="AS57" s="108"/>
+      <c r="AT57" s="108"/>
+      <c r="AU57" s="108"/>
+      <c r="AV57" s="108"/>
+      <c r="AW57" s="108"/>
+      <c r="AX57" s="108"/>
+      <c r="AY57" s="108"/>
+      <c r="AZ57" s="108"/>
+      <c r="BA57" s="108"/>
+      <c r="BB57" s="108"/>
+      <c r="BC57" s="108"/>
+      <c r="BD57" s="108"/>
+      <c r="BE57" s="108"/>
+      <c r="BF57" s="108"/>
+      <c r="BG57" s="108"/>
+      <c r="BH57" s="108"/>
+      <c r="BI57" s="108"/>
+      <c r="BJ57" s="108"/>
+      <c r="BK57" s="108"/>
+      <c r="BL57" s="108"/>
+      <c r="BM57" s="108"/>
+      <c r="BN57" s="108"/>
+    </row>
+    <row r="58" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A58" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>9.1</v>
       </c>
-      <c r="B57" s="81"/>
-      <c r="C57" s="81"/>
-      <c r="D57" s="79"/>
-      <c r="E57" s="100"/>
-      <c r="F57" s="101" t="str">
+      <c r="B58" s="81"/>
+      <c r="C58" s="81"/>
+      <c r="D58" s="79"/>
+      <c r="E58" s="100"/>
+      <c r="F58" s="101" t="str">
         <f t="shared" si="32"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G57" s="62"/>
-      <c r="H57" s="63"/>
-      <c r="I57" s="80" t="str">
+      <c r="G58" s="62"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="80" t="str">
         <f t="shared" si="33"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J57" s="99"/>
-      <c r="K57" s="107"/>
-      <c r="L57" s="107"/>
-      <c r="M57" s="107"/>
-      <c r="N57" s="107"/>
-      <c r="O57" s="107"/>
-      <c r="P57" s="107"/>
-      <c r="Q57" s="107"/>
-      <c r="R57" s="107"/>
-      <c r="S57" s="107"/>
-      <c r="T57" s="107"/>
-      <c r="U57" s="107"/>
-      <c r="V57" s="107"/>
-      <c r="W57" s="107"/>
-      <c r="X57" s="107"/>
-      <c r="Y57" s="107"/>
-      <c r="Z57" s="107"/>
-      <c r="AA57" s="107"/>
-      <c r="AB57" s="107"/>
-      <c r="AC57" s="107"/>
-      <c r="AD57" s="107"/>
-      <c r="AE57" s="107"/>
-      <c r="AF57" s="107"/>
-      <c r="AG57" s="107"/>
-      <c r="AH57" s="107"/>
-      <c r="AI57" s="107"/>
-      <c r="AJ57" s="107"/>
-      <c r="AK57" s="107"/>
-      <c r="AL57" s="107"/>
-      <c r="AM57" s="107"/>
-      <c r="AN57" s="107"/>
-      <c r="AO57" s="107"/>
-      <c r="AP57" s="107"/>
-      <c r="AQ57" s="107"/>
-      <c r="AR57" s="107"/>
-      <c r="AS57" s="107"/>
-      <c r="AT57" s="107"/>
-      <c r="AU57" s="107"/>
-      <c r="AV57" s="107"/>
-      <c r="AW57" s="107"/>
-      <c r="AX57" s="107"/>
-      <c r="AY57" s="107"/>
-      <c r="AZ57" s="107"/>
-      <c r="BA57" s="107"/>
-      <c r="BB57" s="107"/>
-      <c r="BC57" s="107"/>
-      <c r="BD57" s="107"/>
-      <c r="BE57" s="107"/>
-      <c r="BF57" s="107"/>
-      <c r="BG57" s="107"/>
-      <c r="BH57" s="107"/>
-      <c r="BI57" s="107"/>
-      <c r="BJ57" s="107"/>
-      <c r="BK57" s="107"/>
-      <c r="BL57" s="107"/>
-      <c r="BM57" s="107"/>
-      <c r="BN57" s="107"/>
-    </row>
-    <row r="58" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A58" s="53" t="str">
+      <c r="J58" s="99"/>
+      <c r="K58" s="107"/>
+      <c r="L58" s="107"/>
+      <c r="M58" s="107"/>
+      <c r="N58" s="107"/>
+      <c r="O58" s="107"/>
+      <c r="P58" s="107"/>
+      <c r="Q58" s="107"/>
+      <c r="R58" s="107"/>
+      <c r="S58" s="107"/>
+      <c r="T58" s="107"/>
+      <c r="U58" s="107"/>
+      <c r="V58" s="107"/>
+      <c r="W58" s="107"/>
+      <c r="X58" s="107"/>
+      <c r="Y58" s="107"/>
+      <c r="Z58" s="107"/>
+      <c r="AA58" s="107"/>
+      <c r="AB58" s="107"/>
+      <c r="AC58" s="107"/>
+      <c r="AD58" s="107"/>
+      <c r="AE58" s="107"/>
+      <c r="AF58" s="107"/>
+      <c r="AG58" s="107"/>
+      <c r="AH58" s="107"/>
+      <c r="AI58" s="107"/>
+      <c r="AJ58" s="107"/>
+      <c r="AK58" s="107"/>
+      <c r="AL58" s="107"/>
+      <c r="AM58" s="107"/>
+      <c r="AN58" s="107"/>
+      <c r="AO58" s="107"/>
+      <c r="AP58" s="107"/>
+      <c r="AQ58" s="107"/>
+      <c r="AR58" s="107"/>
+      <c r="AS58" s="107"/>
+      <c r="AT58" s="107"/>
+      <c r="AU58" s="107"/>
+      <c r="AV58" s="107"/>
+      <c r="AW58" s="107"/>
+      <c r="AX58" s="107"/>
+      <c r="AY58" s="107"/>
+      <c r="AZ58" s="107"/>
+      <c r="BA58" s="107"/>
+      <c r="BB58" s="107"/>
+      <c r="BC58" s="107"/>
+      <c r="BD58" s="107"/>
+      <c r="BE58" s="107"/>
+      <c r="BF58" s="107"/>
+      <c r="BG58" s="107"/>
+      <c r="BH58" s="107"/>
+      <c r="BI58" s="107"/>
+      <c r="BJ58" s="107"/>
+      <c r="BK58" s="107"/>
+      <c r="BL58" s="107"/>
+      <c r="BM58" s="107"/>
+      <c r="BN58" s="107"/>
+    </row>
+    <row r="59" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A59" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>10</v>
       </c>
-      <c r="B58" s="54" t="s">
+      <c r="B59" s="54" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="56"/>
-      <c r="E58" s="102"/>
-      <c r="F58" s="102" t="str">
+      <c r="D59" s="56"/>
+      <c r="E59" s="102"/>
+      <c r="F59" s="102" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G58" s="57"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="59" t="str">
+      <c r="G59" s="57"/>
+      <c r="H59" s="58"/>
+      <c r="I59" s="59" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J58" s="96"/>
-      <c r="K58" s="108"/>
-      <c r="L58" s="108"/>
-      <c r="M58" s="108"/>
-      <c r="N58" s="108"/>
-      <c r="O58" s="108"/>
-      <c r="P58" s="108"/>
-      <c r="Q58" s="108"/>
-      <c r="R58" s="108"/>
-      <c r="S58" s="108"/>
-      <c r="T58" s="108"/>
-      <c r="U58" s="108"/>
-      <c r="V58" s="108"/>
-      <c r="W58" s="108"/>
-      <c r="X58" s="108"/>
-      <c r="Y58" s="108"/>
-      <c r="Z58" s="108"/>
-      <c r="AA58" s="108"/>
-      <c r="AB58" s="108"/>
-      <c r="AC58" s="108"/>
-      <c r="AD58" s="108"/>
-      <c r="AE58" s="108"/>
-      <c r="AF58" s="108"/>
-      <c r="AG58" s="108"/>
-      <c r="AH58" s="108"/>
-      <c r="AI58" s="108"/>
-      <c r="AJ58" s="108"/>
-      <c r="AK58" s="108"/>
-      <c r="AL58" s="108"/>
-      <c r="AM58" s="108"/>
-      <c r="AN58" s="108"/>
-      <c r="AO58" s="108"/>
-      <c r="AP58" s="108"/>
-      <c r="AQ58" s="108"/>
-      <c r="AR58" s="108"/>
-      <c r="AS58" s="108"/>
-      <c r="AT58" s="108"/>
-      <c r="AU58" s="108"/>
-      <c r="AV58" s="108"/>
-      <c r="AW58" s="108"/>
-      <c r="AX58" s="108"/>
-      <c r="AY58" s="108"/>
-      <c r="AZ58" s="108"/>
-      <c r="BA58" s="108"/>
-      <c r="BB58" s="108"/>
-      <c r="BC58" s="108"/>
-      <c r="BD58" s="108"/>
-      <c r="BE58" s="108"/>
-      <c r="BF58" s="108"/>
-      <c r="BG58" s="108"/>
-      <c r="BH58" s="108"/>
-      <c r="BI58" s="108"/>
-      <c r="BJ58" s="108"/>
-      <c r="BK58" s="108"/>
-      <c r="BL58" s="108"/>
-      <c r="BM58" s="108"/>
-      <c r="BN58" s="108"/>
-    </row>
-    <row r="59" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A59" s="60" t="str">
+      <c r="J59" s="96"/>
+      <c r="K59" s="108"/>
+      <c r="L59" s="108"/>
+      <c r="M59" s="108"/>
+      <c r="N59" s="108"/>
+      <c r="O59" s="108"/>
+      <c r="P59" s="108"/>
+      <c r="Q59" s="108"/>
+      <c r="R59" s="108"/>
+      <c r="S59" s="108"/>
+      <c r="T59" s="108"/>
+      <c r="U59" s="108"/>
+      <c r="V59" s="108"/>
+      <c r="W59" s="108"/>
+      <c r="X59" s="108"/>
+      <c r="Y59" s="108"/>
+      <c r="Z59" s="108"/>
+      <c r="AA59" s="108"/>
+      <c r="AB59" s="108"/>
+      <c r="AC59" s="108"/>
+      <c r="AD59" s="108"/>
+      <c r="AE59" s="108"/>
+      <c r="AF59" s="108"/>
+      <c r="AG59" s="108"/>
+      <c r="AH59" s="108"/>
+      <c r="AI59" s="108"/>
+      <c r="AJ59" s="108"/>
+      <c r="AK59" s="108"/>
+      <c r="AL59" s="108"/>
+      <c r="AM59" s="108"/>
+      <c r="AN59" s="108"/>
+      <c r="AO59" s="108"/>
+      <c r="AP59" s="108"/>
+      <c r="AQ59" s="108"/>
+      <c r="AR59" s="108"/>
+      <c r="AS59" s="108"/>
+      <c r="AT59" s="108"/>
+      <c r="AU59" s="108"/>
+      <c r="AV59" s="108"/>
+      <c r="AW59" s="108"/>
+      <c r="AX59" s="108"/>
+      <c r="AY59" s="108"/>
+      <c r="AZ59" s="108"/>
+      <c r="BA59" s="108"/>
+      <c r="BB59" s="108"/>
+      <c r="BC59" s="108"/>
+      <c r="BD59" s="108"/>
+      <c r="BE59" s="108"/>
+      <c r="BF59" s="108"/>
+      <c r="BG59" s="108"/>
+      <c r="BH59" s="108"/>
+      <c r="BI59" s="108"/>
+      <c r="BJ59" s="108"/>
+      <c r="BK59" s="108"/>
+      <c r="BL59" s="108"/>
+      <c r="BM59" s="108"/>
+      <c r="BN59" s="108"/>
+    </row>
+    <row r="60" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A60" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>10.1</v>
       </c>
-      <c r="B59" s="81"/>
-      <c r="C59" s="81"/>
-      <c r="D59" s="79"/>
-      <c r="E59" s="100"/>
-      <c r="F59" s="101" t="str">
+      <c r="B60" s="81"/>
+      <c r="C60" s="81"/>
+      <c r="D60" s="79"/>
+      <c r="E60" s="100"/>
+      <c r="F60" s="101" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G59" s="62"/>
-      <c r="H59" s="63"/>
-      <c r="I59" s="80" t="str">
+      <c r="G60" s="62"/>
+      <c r="H60" s="63"/>
+      <c r="I60" s="80" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J59" s="99"/>
-      <c r="K59" s="107"/>
-      <c r="L59" s="107"/>
-      <c r="M59" s="107"/>
-      <c r="N59" s="107"/>
-      <c r="O59" s="107"/>
-      <c r="P59" s="107"/>
-      <c r="Q59" s="107"/>
-      <c r="R59" s="107"/>
-      <c r="S59" s="107"/>
-      <c r="T59" s="107"/>
-      <c r="U59" s="107"/>
-      <c r="V59" s="107"/>
-      <c r="W59" s="107"/>
-      <c r="X59" s="107"/>
-      <c r="Y59" s="107"/>
-      <c r="Z59" s="107"/>
-      <c r="AA59" s="107"/>
-      <c r="AB59" s="107"/>
-      <c r="AC59" s="107"/>
-      <c r="AD59" s="107"/>
-      <c r="AE59" s="107"/>
-      <c r="AF59" s="107"/>
-      <c r="AG59" s="107"/>
-      <c r="AH59" s="107"/>
-      <c r="AI59" s="107"/>
-      <c r="AJ59" s="107"/>
-      <c r="AK59" s="107"/>
-      <c r="AL59" s="107"/>
-      <c r="AM59" s="107"/>
-      <c r="AN59" s="107"/>
-      <c r="AO59" s="107"/>
-      <c r="AP59" s="107"/>
-      <c r="AQ59" s="107"/>
-      <c r="AR59" s="107"/>
-      <c r="AS59" s="107"/>
-      <c r="AT59" s="107"/>
-      <c r="AU59" s="107"/>
-      <c r="AV59" s="107"/>
-      <c r="AW59" s="107"/>
-      <c r="AX59" s="107"/>
-      <c r="AY59" s="107"/>
-      <c r="AZ59" s="107"/>
-      <c r="BA59" s="107"/>
-      <c r="BB59" s="107"/>
-      <c r="BC59" s="107"/>
-      <c r="BD59" s="107"/>
-      <c r="BE59" s="107"/>
-      <c r="BF59" s="107"/>
-      <c r="BG59" s="107"/>
-      <c r="BH59" s="107"/>
-      <c r="BI59" s="107"/>
-      <c r="BJ59" s="107"/>
-      <c r="BK59" s="107"/>
-      <c r="BL59" s="107"/>
-      <c r="BM59" s="107"/>
-      <c r="BN59" s="107"/>
-    </row>
-    <row r="60" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A60" s="53" t="str">
+      <c r="J60" s="99"/>
+      <c r="K60" s="107"/>
+      <c r="L60" s="107"/>
+      <c r="M60" s="107"/>
+      <c r="N60" s="107"/>
+      <c r="O60" s="107"/>
+      <c r="P60" s="107"/>
+      <c r="Q60" s="107"/>
+      <c r="R60" s="107"/>
+      <c r="S60" s="107"/>
+      <c r="T60" s="107"/>
+      <c r="U60" s="107"/>
+      <c r="V60" s="107"/>
+      <c r="W60" s="107"/>
+      <c r="X60" s="107"/>
+      <c r="Y60" s="107"/>
+      <c r="Z60" s="107"/>
+      <c r="AA60" s="107"/>
+      <c r="AB60" s="107"/>
+      <c r="AC60" s="107"/>
+      <c r="AD60" s="107"/>
+      <c r="AE60" s="107"/>
+      <c r="AF60" s="107"/>
+      <c r="AG60" s="107"/>
+      <c r="AH60" s="107"/>
+      <c r="AI60" s="107"/>
+      <c r="AJ60" s="107"/>
+      <c r="AK60" s="107"/>
+      <c r="AL60" s="107"/>
+      <c r="AM60" s="107"/>
+      <c r="AN60" s="107"/>
+      <c r="AO60" s="107"/>
+      <c r="AP60" s="107"/>
+      <c r="AQ60" s="107"/>
+      <c r="AR60" s="107"/>
+      <c r="AS60" s="107"/>
+      <c r="AT60" s="107"/>
+      <c r="AU60" s="107"/>
+      <c r="AV60" s="107"/>
+      <c r="AW60" s="107"/>
+      <c r="AX60" s="107"/>
+      <c r="AY60" s="107"/>
+      <c r="AZ60" s="107"/>
+      <c r="BA60" s="107"/>
+      <c r="BB60" s="107"/>
+      <c r="BC60" s="107"/>
+      <c r="BD60" s="107"/>
+      <c r="BE60" s="107"/>
+      <c r="BF60" s="107"/>
+      <c r="BG60" s="107"/>
+      <c r="BH60" s="107"/>
+      <c r="BI60" s="107"/>
+      <c r="BJ60" s="107"/>
+      <c r="BK60" s="107"/>
+      <c r="BL60" s="107"/>
+      <c r="BM60" s="107"/>
+      <c r="BN60" s="107"/>
+    </row>
+    <row r="61" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A61" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>11</v>
       </c>
-      <c r="B60" s="54" t="s">
+      <c r="B61" s="54" t="s">
         <v>156</v>
       </c>
-      <c r="D60" s="56"/>
-      <c r="E60" s="102"/>
-      <c r="F60" s="102" t="str">
+      <c r="D61" s="56"/>
+      <c r="E61" s="102"/>
+      <c r="F61" s="102" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G60" s="57"/>
-      <c r="H60" s="58"/>
-      <c r="I60" s="59" t="str">
+      <c r="G61" s="57"/>
+      <c r="H61" s="58"/>
+      <c r="I61" s="59" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J60" s="96"/>
-      <c r="K60" s="108"/>
-      <c r="L60" s="108"/>
-      <c r="M60" s="108"/>
-      <c r="N60" s="108"/>
-      <c r="O60" s="108"/>
-      <c r="P60" s="108"/>
-      <c r="Q60" s="108"/>
-      <c r="R60" s="108"/>
-      <c r="S60" s="108"/>
-      <c r="T60" s="108"/>
-      <c r="U60" s="108"/>
-      <c r="V60" s="108"/>
-      <c r="W60" s="108"/>
-      <c r="X60" s="108"/>
-      <c r="Y60" s="108"/>
-      <c r="Z60" s="108"/>
-      <c r="AA60" s="108"/>
-      <c r="AB60" s="108"/>
-      <c r="AC60" s="108"/>
-      <c r="AD60" s="108"/>
-      <c r="AE60" s="108"/>
-      <c r="AF60" s="108"/>
-      <c r="AG60" s="108"/>
-      <c r="AH60" s="108"/>
-      <c r="AI60" s="108"/>
-      <c r="AJ60" s="108"/>
-      <c r="AK60" s="108"/>
-      <c r="AL60" s="108"/>
-      <c r="AM60" s="108"/>
-      <c r="AN60" s="108"/>
-      <c r="AO60" s="108"/>
-      <c r="AP60" s="108"/>
-      <c r="AQ60" s="108"/>
-      <c r="AR60" s="108"/>
-      <c r="AS60" s="108"/>
-      <c r="AT60" s="108"/>
-      <c r="AU60" s="108"/>
-      <c r="AV60" s="108"/>
-      <c r="AW60" s="108"/>
-      <c r="AX60" s="108"/>
-      <c r="AY60" s="108"/>
-      <c r="AZ60" s="108"/>
-      <c r="BA60" s="108"/>
-      <c r="BB60" s="108"/>
-      <c r="BC60" s="108"/>
-      <c r="BD60" s="108"/>
-      <c r="BE60" s="108"/>
-      <c r="BF60" s="108"/>
-      <c r="BG60" s="108"/>
-      <c r="BH60" s="108"/>
-      <c r="BI60" s="108"/>
-      <c r="BJ60" s="108"/>
-      <c r="BK60" s="108"/>
-      <c r="BL60" s="108"/>
-      <c r="BM60" s="108"/>
-      <c r="BN60" s="108"/>
-    </row>
-    <row r="61" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A61" s="60" t="str">
+      <c r="J61" s="96"/>
+      <c r="K61" s="108"/>
+      <c r="L61" s="108"/>
+      <c r="M61" s="108"/>
+      <c r="N61" s="108"/>
+      <c r="O61" s="108"/>
+      <c r="P61" s="108"/>
+      <c r="Q61" s="108"/>
+      <c r="R61" s="108"/>
+      <c r="S61" s="108"/>
+      <c r="T61" s="108"/>
+      <c r="U61" s="108"/>
+      <c r="V61" s="108"/>
+      <c r="W61" s="108"/>
+      <c r="X61" s="108"/>
+      <c r="Y61" s="108"/>
+      <c r="Z61" s="108"/>
+      <c r="AA61" s="108"/>
+      <c r="AB61" s="108"/>
+      <c r="AC61" s="108"/>
+      <c r="AD61" s="108"/>
+      <c r="AE61" s="108"/>
+      <c r="AF61" s="108"/>
+      <c r="AG61" s="108"/>
+      <c r="AH61" s="108"/>
+      <c r="AI61" s="108"/>
+      <c r="AJ61" s="108"/>
+      <c r="AK61" s="108"/>
+      <c r="AL61" s="108"/>
+      <c r="AM61" s="108"/>
+      <c r="AN61" s="108"/>
+      <c r="AO61" s="108"/>
+      <c r="AP61" s="108"/>
+      <c r="AQ61" s="108"/>
+      <c r="AR61" s="108"/>
+      <c r="AS61" s="108"/>
+      <c r="AT61" s="108"/>
+      <c r="AU61" s="108"/>
+      <c r="AV61" s="108"/>
+      <c r="AW61" s="108"/>
+      <c r="AX61" s="108"/>
+      <c r="AY61" s="108"/>
+      <c r="AZ61" s="108"/>
+      <c r="BA61" s="108"/>
+      <c r="BB61" s="108"/>
+      <c r="BC61" s="108"/>
+      <c r="BD61" s="108"/>
+      <c r="BE61" s="108"/>
+      <c r="BF61" s="108"/>
+      <c r="BG61" s="108"/>
+      <c r="BH61" s="108"/>
+      <c r="BI61" s="108"/>
+      <c r="BJ61" s="108"/>
+      <c r="BK61" s="108"/>
+      <c r="BL61" s="108"/>
+      <c r="BM61" s="108"/>
+      <c r="BN61" s="108"/>
+    </row>
+    <row r="62" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A62" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>11.1</v>
       </c>
-      <c r="B61" s="81"/>
-      <c r="C61" s="81"/>
-      <c r="D61" s="79"/>
-      <c r="E61" s="100"/>
-      <c r="F61" s="101" t="str">
+      <c r="B62" s="81"/>
+      <c r="C62" s="81"/>
+      <c r="D62" s="79"/>
+      <c r="E62" s="100"/>
+      <c r="F62" s="101" t="str">
         <f t="shared" si="28"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G61" s="62"/>
-      <c r="H61" s="63"/>
-      <c r="I61" s="80" t="str">
+      <c r="G62" s="62"/>
+      <c r="H62" s="63"/>
+      <c r="I62" s="80" t="str">
         <f t="shared" si="29"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J61" s="99"/>
-      <c r="K61" s="107"/>
-      <c r="L61" s="107"/>
-      <c r="M61" s="107"/>
-      <c r="N61" s="107"/>
-      <c r="O61" s="107"/>
-      <c r="P61" s="107"/>
-      <c r="Q61" s="107"/>
-      <c r="R61" s="107"/>
-      <c r="S61" s="107"/>
-      <c r="T61" s="107"/>
-      <c r="U61" s="107"/>
-      <c r="V61" s="107"/>
-      <c r="W61" s="107"/>
-      <c r="X61" s="107"/>
-      <c r="Y61" s="107"/>
-      <c r="Z61" s="107"/>
-      <c r="AA61" s="107"/>
-      <c r="AB61" s="107"/>
-      <c r="AC61" s="107"/>
-      <c r="AD61" s="107"/>
-      <c r="AE61" s="107"/>
-      <c r="AF61" s="107"/>
-      <c r="AG61" s="107"/>
-      <c r="AH61" s="107"/>
-      <c r="AI61" s="107"/>
-      <c r="AJ61" s="107"/>
-      <c r="AK61" s="107"/>
-      <c r="AL61" s="107"/>
-      <c r="AM61" s="107"/>
-      <c r="AN61" s="107"/>
-      <c r="AO61" s="107"/>
-      <c r="AP61" s="107"/>
-      <c r="AQ61" s="107"/>
-      <c r="AR61" s="107"/>
-      <c r="AS61" s="107"/>
-      <c r="AT61" s="107"/>
-      <c r="AU61" s="107"/>
-      <c r="AV61" s="107"/>
-      <c r="AW61" s="107"/>
-      <c r="AX61" s="107"/>
-      <c r="AY61" s="107"/>
-      <c r="AZ61" s="107"/>
-      <c r="BA61" s="107"/>
-      <c r="BB61" s="107"/>
-      <c r="BC61" s="107"/>
-      <c r="BD61" s="107"/>
-      <c r="BE61" s="107"/>
-      <c r="BF61" s="107"/>
-      <c r="BG61" s="107"/>
-      <c r="BH61" s="107"/>
-      <c r="BI61" s="107"/>
-      <c r="BJ61" s="107"/>
-      <c r="BK61" s="107"/>
-      <c r="BL61" s="107"/>
-      <c r="BM61" s="107"/>
-      <c r="BN61" s="107"/>
-    </row>
-    <row r="62" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A62" s="53" t="str">
+      <c r="J62" s="99"/>
+      <c r="K62" s="107"/>
+      <c r="L62" s="107"/>
+      <c r="M62" s="107"/>
+      <c r="N62" s="107"/>
+      <c r="O62" s="107"/>
+      <c r="P62" s="107"/>
+      <c r="Q62" s="107"/>
+      <c r="R62" s="107"/>
+      <c r="S62" s="107"/>
+      <c r="T62" s="107"/>
+      <c r="U62" s="107"/>
+      <c r="V62" s="107"/>
+      <c r="W62" s="107"/>
+      <c r="X62" s="107"/>
+      <c r="Y62" s="107"/>
+      <c r="Z62" s="107"/>
+      <c r="AA62" s="107"/>
+      <c r="AB62" s="107"/>
+      <c r="AC62" s="107"/>
+      <c r="AD62" s="107"/>
+      <c r="AE62" s="107"/>
+      <c r="AF62" s="107"/>
+      <c r="AG62" s="107"/>
+      <c r="AH62" s="107"/>
+      <c r="AI62" s="107"/>
+      <c r="AJ62" s="107"/>
+      <c r="AK62" s="107"/>
+      <c r="AL62" s="107"/>
+      <c r="AM62" s="107"/>
+      <c r="AN62" s="107"/>
+      <c r="AO62" s="107"/>
+      <c r="AP62" s="107"/>
+      <c r="AQ62" s="107"/>
+      <c r="AR62" s="107"/>
+      <c r="AS62" s="107"/>
+      <c r="AT62" s="107"/>
+      <c r="AU62" s="107"/>
+      <c r="AV62" s="107"/>
+      <c r="AW62" s="107"/>
+      <c r="AX62" s="107"/>
+      <c r="AY62" s="107"/>
+      <c r="AZ62" s="107"/>
+      <c r="BA62" s="107"/>
+      <c r="BB62" s="107"/>
+      <c r="BC62" s="107"/>
+      <c r="BD62" s="107"/>
+      <c r="BE62" s="107"/>
+      <c r="BF62" s="107"/>
+      <c r="BG62" s="107"/>
+      <c r="BH62" s="107"/>
+      <c r="BI62" s="107"/>
+      <c r="BJ62" s="107"/>
+      <c r="BK62" s="107"/>
+      <c r="BL62" s="107"/>
+      <c r="BM62" s="107"/>
+      <c r="BN62" s="107"/>
+    </row>
+    <row r="63" spans="1:66" s="55" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A63" s="53" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>12</v>
       </c>
-      <c r="B62" s="54" t="s">
+      <c r="B63" s="54" t="s">
         <v>157</v>
       </c>
-      <c r="D62" s="56"/>
-      <c r="E62" s="102"/>
-      <c r="F62" s="102" t="str">
-        <f t="shared" ref="F62:F63" si="34">IF(ISBLANK(E62)," - ",IF(G62=0,E62,E62+G62-1))</f>
+      <c r="D63" s="56"/>
+      <c r="E63" s="102"/>
+      <c r="F63" s="102" t="str">
+        <f t="shared" ref="F63:F64" si="34">IF(ISBLANK(E63)," - ",IF(G63=0,E63,E63+G63-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G62" s="57"/>
-      <c r="H62" s="58"/>
-      <c r="I62" s="59" t="str">
-        <f t="shared" ref="I62:I63" si="35">IF(OR(F62=0,E62=0)," - ",NETWORKDAYS(E62,F62))</f>
+      <c r="G63" s="57"/>
+      <c r="H63" s="58"/>
+      <c r="I63" s="59" t="str">
+        <f t="shared" ref="I63:I64" si="35">IF(OR(F63=0,E63=0)," - ",NETWORKDAYS(E63,F63))</f>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J62" s="96"/>
-      <c r="K62" s="108"/>
-      <c r="L62" s="108"/>
-      <c r="M62" s="108"/>
-      <c r="N62" s="108"/>
-      <c r="O62" s="108"/>
-      <c r="P62" s="108"/>
-      <c r="Q62" s="108"/>
-      <c r="R62" s="108"/>
-      <c r="S62" s="108"/>
-      <c r="T62" s="108"/>
-      <c r="U62" s="108"/>
-      <c r="V62" s="108"/>
-      <c r="W62" s="108"/>
-      <c r="X62" s="108"/>
-      <c r="Y62" s="108"/>
-      <c r="Z62" s="108"/>
-      <c r="AA62" s="108"/>
-      <c r="AB62" s="108"/>
-      <c r="AC62" s="108"/>
-      <c r="AD62" s="108"/>
-      <c r="AE62" s="108"/>
-      <c r="AF62" s="108"/>
-      <c r="AG62" s="108"/>
-      <c r="AH62" s="108"/>
-      <c r="AI62" s="108"/>
-      <c r="AJ62" s="108"/>
-      <c r="AK62" s="108"/>
-      <c r="AL62" s="108"/>
-      <c r="AM62" s="108"/>
-      <c r="AN62" s="108"/>
-      <c r="AO62" s="108"/>
-      <c r="AP62" s="108"/>
-      <c r="AQ62" s="108"/>
-      <c r="AR62" s="108"/>
-      <c r="AS62" s="108"/>
-      <c r="AT62" s="108"/>
-      <c r="AU62" s="108"/>
-      <c r="AV62" s="108"/>
-      <c r="AW62" s="108"/>
-      <c r="AX62" s="108"/>
-      <c r="AY62" s="108"/>
-      <c r="AZ62" s="108"/>
-      <c r="BA62" s="108"/>
-      <c r="BB62" s="108"/>
-      <c r="BC62" s="108"/>
-      <c r="BD62" s="108"/>
-      <c r="BE62" s="108"/>
-      <c r="BF62" s="108"/>
-      <c r="BG62" s="108"/>
-      <c r="BH62" s="108"/>
-      <c r="BI62" s="108"/>
-      <c r="BJ62" s="108"/>
-      <c r="BK62" s="108"/>
-      <c r="BL62" s="108"/>
-      <c r="BM62" s="108"/>
-      <c r="BN62" s="108"/>
-    </row>
-    <row r="63" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A63" s="60" t="str">
+      <c r="J63" s="96"/>
+      <c r="K63" s="108"/>
+      <c r="L63" s="108"/>
+      <c r="M63" s="108"/>
+      <c r="N63" s="108"/>
+      <c r="O63" s="108"/>
+      <c r="P63" s="108"/>
+      <c r="Q63" s="108"/>
+      <c r="R63" s="108"/>
+      <c r="S63" s="108"/>
+      <c r="T63" s="108"/>
+      <c r="U63" s="108"/>
+      <c r="V63" s="108"/>
+      <c r="W63" s="108"/>
+      <c r="X63" s="108"/>
+      <c r="Y63" s="108"/>
+      <c r="Z63" s="108"/>
+      <c r="AA63" s="108"/>
+      <c r="AB63" s="108"/>
+      <c r="AC63" s="108"/>
+      <c r="AD63" s="108"/>
+      <c r="AE63" s="108"/>
+      <c r="AF63" s="108"/>
+      <c r="AG63" s="108"/>
+      <c r="AH63" s="108"/>
+      <c r="AI63" s="108"/>
+      <c r="AJ63" s="108"/>
+      <c r="AK63" s="108"/>
+      <c r="AL63" s="108"/>
+      <c r="AM63" s="108"/>
+      <c r="AN63" s="108"/>
+      <c r="AO63" s="108"/>
+      <c r="AP63" s="108"/>
+      <c r="AQ63" s="108"/>
+      <c r="AR63" s="108"/>
+      <c r="AS63" s="108"/>
+      <c r="AT63" s="108"/>
+      <c r="AU63" s="108"/>
+      <c r="AV63" s="108"/>
+      <c r="AW63" s="108"/>
+      <c r="AX63" s="108"/>
+      <c r="AY63" s="108"/>
+      <c r="AZ63" s="108"/>
+      <c r="BA63" s="108"/>
+      <c r="BB63" s="108"/>
+      <c r="BC63" s="108"/>
+      <c r="BD63" s="108"/>
+      <c r="BE63" s="108"/>
+      <c r="BF63" s="108"/>
+      <c r="BG63" s="108"/>
+      <c r="BH63" s="108"/>
+      <c r="BI63" s="108"/>
+      <c r="BJ63" s="108"/>
+      <c r="BK63" s="108"/>
+      <c r="BL63" s="108"/>
+      <c r="BM63" s="108"/>
+      <c r="BN63" s="108"/>
+    </row>
+    <row r="64" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A64" s="60" t="str">
         <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>12.1</v>
       </c>
-      <c r="B63" s="81"/>
-      <c r="C63" s="81"/>
-      <c r="D63" s="79"/>
-      <c r="E63" s="100"/>
-      <c r="F63" s="101" t="str">
+      <c r="B64" s="81"/>
+      <c r="C64" s="81"/>
+      <c r="D64" s="79"/>
+      <c r="E64" s="100"/>
+      <c r="F64" s="101" t="str">
         <f t="shared" si="34"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="G63" s="62"/>
-      <c r="H63" s="63"/>
-      <c r="I63" s="80" t="str">
+      <c r="G64" s="62"/>
+      <c r="H64" s="63"/>
+      <c r="I64" s="80" t="str">
         <f t="shared" si="35"/>
         <v xml:space="preserve"> - </v>
       </c>
-      <c r="J63" s="99"/>
-      <c r="K63" s="107"/>
-      <c r="L63" s="107"/>
-      <c r="M63" s="107"/>
-      <c r="N63" s="107"/>
-      <c r="O63" s="107"/>
-      <c r="P63" s="107"/>
-      <c r="Q63" s="107"/>
-      <c r="R63" s="107"/>
-      <c r="S63" s="107"/>
-      <c r="T63" s="107"/>
-      <c r="U63" s="107"/>
-      <c r="V63" s="107"/>
-      <c r="W63" s="107"/>
-      <c r="X63" s="107"/>
-      <c r="Y63" s="107"/>
-      <c r="Z63" s="107"/>
-      <c r="AA63" s="107"/>
-      <c r="AB63" s="107"/>
-      <c r="AC63" s="107"/>
-      <c r="AD63" s="107"/>
-      <c r="AE63" s="107"/>
-      <c r="AF63" s="107"/>
-      <c r="AG63" s="107"/>
-      <c r="AH63" s="107"/>
-      <c r="AI63" s="107"/>
-      <c r="AJ63" s="107"/>
-      <c r="AK63" s="107"/>
-      <c r="AL63" s="107"/>
-      <c r="AM63" s="107"/>
-      <c r="AN63" s="107"/>
-      <c r="AO63" s="107"/>
-      <c r="AP63" s="107"/>
-      <c r="AQ63" s="107"/>
-      <c r="AR63" s="107"/>
-      <c r="AS63" s="107"/>
-      <c r="AT63" s="107"/>
-      <c r="AU63" s="107"/>
-      <c r="AV63" s="107"/>
-      <c r="AW63" s="107"/>
-      <c r="AX63" s="107"/>
-      <c r="AY63" s="107"/>
-      <c r="AZ63" s="107"/>
-      <c r="BA63" s="107"/>
-      <c r="BB63" s="107"/>
-      <c r="BC63" s="107"/>
-      <c r="BD63" s="107"/>
-      <c r="BE63" s="107"/>
-      <c r="BF63" s="107"/>
-      <c r="BG63" s="107"/>
-      <c r="BH63" s="107"/>
-      <c r="BI63" s="107"/>
-      <c r="BJ63" s="107"/>
-      <c r="BK63" s="107"/>
-      <c r="BL63" s="107"/>
-      <c r="BM63" s="107"/>
-      <c r="BN63" s="107"/>
-    </row>
-    <row r="64" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A64" s="60"/>
-      <c r="B64" s="65"/>
-      <c r="C64" s="65"/>
-      <c r="D64" s="66"/>
-      <c r="E64" s="103"/>
-      <c r="F64" s="103"/>
-      <c r="G64" s="67"/>
-      <c r="H64" s="68"/>
-      <c r="I64" s="69" t="str">
-        <f t="shared" si="4"/>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J64" s="97"/>
+      <c r="J64" s="99"/>
       <c r="K64" s="107"/>
       <c r="L64" s="107"/>
       <c r="M64" s="107"/>
@@ -9602,19 +9703,20 @@
       <c r="BM64" s="107"/>
       <c r="BN64" s="107"/>
     </row>
-    <row r="65" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A65" s="71" t="s">
-        <v>1</v>
-      </c>
-      <c r="B65" s="72"/>
-      <c r="C65" s="73"/>
-      <c r="D65" s="73"/>
-      <c r="E65" s="104"/>
-      <c r="F65" s="104"/>
-      <c r="G65" s="74"/>
-      <c r="H65" s="74"/>
-      <c r="I65" s="74"/>
-      <c r="J65" s="98"/>
+    <row r="65" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A65" s="60"/>
+      <c r="B65" s="65"/>
+      <c r="C65" s="65"/>
+      <c r="D65" s="66"/>
+      <c r="E65" s="103"/>
+      <c r="F65" s="103"/>
+      <c r="G65" s="67"/>
+      <c r="H65" s="68"/>
+      <c r="I65" s="69" t="str">
+        <f t="shared" si="4"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J65" s="97"/>
       <c r="K65" s="107"/>
       <c r="L65" s="107"/>
       <c r="M65" s="107"/>
@@ -9672,18 +9774,18 @@
       <c r="BM65" s="107"/>
       <c r="BN65" s="107"/>
     </row>
-    <row r="66" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A66" s="76" t="s">
-        <v>37</v>
-      </c>
-      <c r="B66" s="77"/>
-      <c r="C66" s="77"/>
-      <c r="D66" s="77"/>
-      <c r="E66" s="105"/>
-      <c r="F66" s="105"/>
-      <c r="G66" s="77"/>
-      <c r="H66" s="77"/>
-      <c r="I66" s="77"/>
+    <row r="66" spans="1:66" s="75" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A66" s="71" t="s">
+        <v>1</v>
+      </c>
+      <c r="B66" s="72"/>
+      <c r="C66" s="73"/>
+      <c r="D66" s="73"/>
+      <c r="E66" s="104"/>
+      <c r="F66" s="104"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
       <c r="J66" s="98"/>
       <c r="K66" s="107"/>
       <c r="L66" s="107"/>
@@ -9743,27 +9845,18 @@
       <c r="BN66" s="107"/>
     </row>
     <row r="67" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A67" s="127" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
-        <v>1</v>
-      </c>
-      <c r="B67" s="128" t="s">
-        <v>76</v>
-      </c>
-      <c r="C67" s="78"/>
-      <c r="D67" s="79"/>
-      <c r="E67" s="100"/>
-      <c r="F67" s="101" t="str">
-        <f t="shared" ref="F67:F70" si="36">IF(ISBLANK(E67)," - ",IF(G67=0,E67,E67+G67-1))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="G67" s="62"/>
-      <c r="H67" s="63"/>
-      <c r="I67" s="80" t="str">
-        <f>IF(OR(F67=0,E67=0)," - ",NETWORKDAYS(E67,F67))</f>
-        <v xml:space="preserve"> - </v>
-      </c>
-      <c r="J67" s="99"/>
+      <c r="A67" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" s="77"/>
+      <c r="C67" s="77"/>
+      <c r="D67" s="77"/>
+      <c r="E67" s="105"/>
+      <c r="F67" s="105"/>
+      <c r="G67" s="77"/>
+      <c r="H67" s="77"/>
+      <c r="I67" s="77"/>
+      <c r="J67" s="98"/>
       <c r="K67" s="107"/>
       <c r="L67" s="107"/>
       <c r="M67" s="107"/>
@@ -9822,24 +9915,24 @@
       <c r="BN67" s="107"/>
     </row>
     <row r="68" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A68" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
-        <v>1.1</v>
-      </c>
-      <c r="B68" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="C68" s="81"/>
+      <c r="A68" s="127" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <v>1</v>
+      </c>
+      <c r="B68" s="128" t="s">
+        <v>76</v>
+      </c>
+      <c r="C68" s="78"/>
       <c r="D68" s="79"/>
       <c r="E68" s="100"/>
       <c r="F68" s="101" t="str">
-        <f t="shared" si="36"/>
+        <f t="shared" ref="F68:F71" si="36">IF(ISBLANK(E68)," - ",IF(G68=0,E68,E68+G68-1))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="G68" s="62"/>
       <c r="H68" s="63"/>
       <c r="I68" s="80" t="str">
-        <f t="shared" ref="I68:I70" si="37">IF(OR(F68=0,E68=0)," - ",NETWORKDAYS(E68,F68))</f>
+        <f>IF(OR(F68=0,E68=0)," - ",NETWORKDAYS(E68,F68))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J68" s="99"/>
@@ -9902,11 +9995,11 @@
     </row>
     <row r="69" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A69" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
-        <v>1.1.1</v>
-      </c>
-      <c r="B69" s="82" t="s">
-        <v>63</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <v>1.1</v>
+      </c>
+      <c r="B69" s="81" t="s">
+        <v>62</v>
       </c>
       <c r="C69" s="81"/>
       <c r="D69" s="79"/>
@@ -9918,7 +10011,7 @@
       <c r="G69" s="62"/>
       <c r="H69" s="63"/>
       <c r="I69" s="80" t="str">
-        <f t="shared" si="37"/>
+        <f t="shared" ref="I69:I71" si="37">IF(OR(F69=0,E69=0)," - ",NETWORKDAYS(E69,F69))</f>
         <v xml:space="preserve"> - </v>
       </c>
       <c r="J69" s="99"/>
@@ -9981,11 +10074,11 @@
     </row>
     <row r="70" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
       <c r="A70" s="60" t="str">
-        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
-        <v>1.1.1.1</v>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <v>1.1.1</v>
       </c>
       <c r="B70" s="82" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C70" s="81"/>
       <c r="D70" s="79"/>
@@ -10058,77 +10151,165 @@
       <c r="BM70" s="107"/>
       <c r="BN70" s="107"/>
     </row>
-    <row r="71" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A71" s="30"/>
-      <c r="B71" s="31"/>
-      <c r="C71" s="31"/>
-      <c r="D71" s="32"/>
-      <c r="E71" s="31"/>
-      <c r="F71" s="31"/>
-      <c r="G71" s="31"/>
-      <c r="H71" s="31"/>
-      <c r="I71" s="31"/>
-      <c r="J71" s="31"/>
-      <c r="K71" s="31"/>
-      <c r="L71" s="31"/>
-      <c r="M71" s="31"/>
-      <c r="N71" s="31"/>
-      <c r="O71" s="31"/>
-      <c r="P71" s="31"/>
-      <c r="Q71" s="31"/>
-      <c r="R71" s="31"/>
-      <c r="S71" s="31"/>
-      <c r="T71" s="31"/>
-      <c r="U71" s="31"/>
-      <c r="V71" s="31"/>
-      <c r="W71" s="31"/>
-      <c r="X71" s="31"/>
-      <c r="Y71" s="31"/>
-      <c r="Z71" s="31"/>
-      <c r="AA71" s="31"/>
-      <c r="AB71" s="31"/>
-      <c r="AC71" s="31"/>
-      <c r="AD71" s="31"/>
-      <c r="AE71" s="31"/>
-      <c r="AF71" s="31"/>
-      <c r="AG71" s="31"/>
-      <c r="AH71" s="31"/>
-      <c r="AI71" s="31"/>
-      <c r="AJ71" s="31"/>
-      <c r="AK71" s="31"/>
-      <c r="AL71" s="31"/>
-      <c r="AM71" s="31"/>
-      <c r="AN71" s="31"/>
-      <c r="AO71" s="31"/>
-      <c r="AP71" s="31"/>
-      <c r="AQ71" s="31"/>
-      <c r="AR71" s="31"/>
-      <c r="AS71" s="31"/>
-      <c r="AT71" s="31"/>
-      <c r="AU71" s="31"/>
-      <c r="AV71" s="31"/>
-      <c r="AW71" s="31"/>
-      <c r="AX71" s="31"/>
-      <c r="AY71" s="31"/>
-      <c r="AZ71" s="31"/>
-      <c r="BA71" s="31"/>
-      <c r="BB71" s="31"/>
-      <c r="BC71" s="31"/>
-      <c r="BD71" s="31"/>
-      <c r="BE71" s="31"/>
-      <c r="BF71" s="31"/>
-      <c r="BG71" s="31"/>
-      <c r="BH71" s="31"/>
-      <c r="BI71" s="31"/>
-      <c r="BJ71" s="31"/>
-      <c r="BK71" s="31"/>
-      <c r="BL71" s="31"/>
-      <c r="BM71" s="31"/>
-      <c r="BN71" s="31"/>
+    <row r="71" spans="1:66" s="70" customFormat="1" ht="18" x14ac:dyDescent="0.15">
+      <c r="A71" s="60" t="str">
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <v>1.1.1.1</v>
+      </c>
+      <c r="B71" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="C71" s="81"/>
+      <c r="D71" s="79"/>
+      <c r="E71" s="100"/>
+      <c r="F71" s="101" t="str">
+        <f t="shared" si="36"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="G71" s="62"/>
+      <c r="H71" s="63"/>
+      <c r="I71" s="80" t="str">
+        <f t="shared" si="37"/>
+        <v xml:space="preserve"> - </v>
+      </c>
+      <c r="J71" s="99"/>
+      <c r="K71" s="107"/>
+      <c r="L71" s="107"/>
+      <c r="M71" s="107"/>
+      <c r="N71" s="107"/>
+      <c r="O71" s="107"/>
+      <c r="P71" s="107"/>
+      <c r="Q71" s="107"/>
+      <c r="R71" s="107"/>
+      <c r="S71" s="107"/>
+      <c r="T71" s="107"/>
+      <c r="U71" s="107"/>
+      <c r="V71" s="107"/>
+      <c r="W71" s="107"/>
+      <c r="X71" s="107"/>
+      <c r="Y71" s="107"/>
+      <c r="Z71" s="107"/>
+      <c r="AA71" s="107"/>
+      <c r="AB71" s="107"/>
+      <c r="AC71" s="107"/>
+      <c r="AD71" s="107"/>
+      <c r="AE71" s="107"/>
+      <c r="AF71" s="107"/>
+      <c r="AG71" s="107"/>
+      <c r="AH71" s="107"/>
+      <c r="AI71" s="107"/>
+      <c r="AJ71" s="107"/>
+      <c r="AK71" s="107"/>
+      <c r="AL71" s="107"/>
+      <c r="AM71" s="107"/>
+      <c r="AN71" s="107"/>
+      <c r="AO71" s="107"/>
+      <c r="AP71" s="107"/>
+      <c r="AQ71" s="107"/>
+      <c r="AR71" s="107"/>
+      <c r="AS71" s="107"/>
+      <c r="AT71" s="107"/>
+      <c r="AU71" s="107"/>
+      <c r="AV71" s="107"/>
+      <c r="AW71" s="107"/>
+      <c r="AX71" s="107"/>
+      <c r="AY71" s="107"/>
+      <c r="AZ71" s="107"/>
+      <c r="BA71" s="107"/>
+      <c r="BB71" s="107"/>
+      <c r="BC71" s="107"/>
+      <c r="BD71" s="107"/>
+      <c r="BE71" s="107"/>
+      <c r="BF71" s="107"/>
+      <c r="BG71" s="107"/>
+      <c r="BH71" s="107"/>
+      <c r="BI71" s="107"/>
+      <c r="BJ71" s="107"/>
+      <c r="BK71" s="107"/>
+      <c r="BL71" s="107"/>
+      <c r="BM71" s="107"/>
+      <c r="BN71" s="107"/>
+    </row>
+    <row r="72" spans="1:66" s="33" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="30"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="31"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="31"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="31"/>
+      <c r="K72" s="31"/>
+      <c r="L72" s="31"/>
+      <c r="M72" s="31"/>
+      <c r="N72" s="31"/>
+      <c r="O72" s="31"/>
+      <c r="P72" s="31"/>
+      <c r="Q72" s="31"/>
+      <c r="R72" s="31"/>
+      <c r="S72" s="31"/>
+      <c r="T72" s="31"/>
+      <c r="U72" s="31"/>
+      <c r="V72" s="31"/>
+      <c r="W72" s="31"/>
+      <c r="X72" s="31"/>
+      <c r="Y72" s="31"/>
+      <c r="Z72" s="31"/>
+      <c r="AA72" s="31"/>
+      <c r="AB72" s="31"/>
+      <c r="AC72" s="31"/>
+      <c r="AD72" s="31"/>
+      <c r="AE72" s="31"/>
+      <c r="AF72" s="31"/>
+      <c r="AG72" s="31"/>
+      <c r="AH72" s="31"/>
+      <c r="AI72" s="31"/>
+      <c r="AJ72" s="31"/>
+      <c r="AK72" s="31"/>
+      <c r="AL72" s="31"/>
+      <c r="AM72" s="31"/>
+      <c r="AN72" s="31"/>
+      <c r="AO72" s="31"/>
+      <c r="AP72" s="31"/>
+      <c r="AQ72" s="31"/>
+      <c r="AR72" s="31"/>
+      <c r="AS72" s="31"/>
+      <c r="AT72" s="31"/>
+      <c r="AU72" s="31"/>
+      <c r="AV72" s="31"/>
+      <c r="AW72" s="31"/>
+      <c r="AX72" s="31"/>
+      <c r="AY72" s="31"/>
+      <c r="AZ72" s="31"/>
+      <c r="BA72" s="31"/>
+      <c r="BB72" s="31"/>
+      <c r="BC72" s="31"/>
+      <c r="BD72" s="31"/>
+      <c r="BE72" s="31"/>
+      <c r="BF72" s="31"/>
+      <c r="BG72" s="31"/>
+      <c r="BH72" s="31"/>
+      <c r="BI72" s="31"/>
+      <c r="BJ72" s="31"/>
+      <c r="BK72" s="31"/>
+      <c r="BL72" s="31"/>
+      <c r="BM72" s="31"/>
+      <c r="BN72" s="31"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -10139,19 +10320,10 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="H8:H11 H16:H18 H64:H70 H30 H20:H28 H13">
-    <cfRule type="dataBar" priority="194">
+  <conditionalFormatting sqref="H8:H11 H16:H18 H65:H71 H30 H20:H28 H13">
+    <cfRule type="dataBar" priority="198">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10165,25 +10337,25 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:BN7">
-    <cfRule type="expression" dxfId="65" priority="237">
+    <cfRule type="expression" dxfId="71" priority="241">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K8:BN11 K13:BN18 K20:BN30 K33:BN34 K40:BN70">
-    <cfRule type="expression" dxfId="64" priority="240">
+  <conditionalFormatting sqref="K8:BN11 K13:BN18 K20:BN30 K33:BN34 K40:BN53 K55:BN71">
+    <cfRule type="expression" dxfId="70" priority="244">
       <formula>AND($E8&lt;=K$6,ROUNDDOWN(($F8-$E8+1)*$H8,0)+$E8-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="241">
+    <cfRule type="expression" dxfId="69" priority="245">
       <formula>AND(NOT(ISBLANK($E8)),$E8&lt;=K$6,$F8&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:BN11 K16:BN18 K64:BN70 K30:BN30 K20:BN28 K13:BN13">
-    <cfRule type="expression" dxfId="62" priority="200">
+  <conditionalFormatting sqref="K6:BN11 K16:BN18 K65:BN71 K30:BN30 K20:BN28 K13:BN13">
+    <cfRule type="expression" dxfId="68" priority="204">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H15">
-    <cfRule type="dataBar" priority="178">
+    <cfRule type="dataBar" priority="182">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10197,17 +10369,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K15:BN15">
-    <cfRule type="expression" dxfId="61" priority="185">
+    <cfRule type="expression" dxfId="67" priority="189">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K14:BN14">
-    <cfRule type="expression" dxfId="60" priority="181">
+    <cfRule type="expression" dxfId="66" priority="185">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H14">
-    <cfRule type="dataBar" priority="179">
+    <cfRule type="dataBar" priority="183">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10221,7 +10393,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H33">
-    <cfRule type="dataBar" priority="171">
+    <cfRule type="dataBar" priority="175">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10235,12 +10407,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K33:BN33">
-    <cfRule type="expression" dxfId="59" priority="172">
+    <cfRule type="expression" dxfId="65" priority="176">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H34">
-    <cfRule type="dataBar" priority="163">
+    <cfRule type="dataBar" priority="167">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10254,7 +10426,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41">
-    <cfRule type="dataBar" priority="155">
+    <cfRule type="dataBar" priority="159">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10268,12 +10440,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K34:BN34">
-    <cfRule type="expression" dxfId="58" priority="164">
+    <cfRule type="expression" dxfId="64" priority="168">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H55">
-    <cfRule type="dataBar" priority="147">
+  <conditionalFormatting sqref="H56">
+    <cfRule type="dataBar" priority="151">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10287,12 +10459,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K41:BN41">
-    <cfRule type="expression" dxfId="57" priority="156">
+    <cfRule type="expression" dxfId="63" priority="160">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="dataBar" priority="159">
+    <cfRule type="dataBar" priority="163">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10306,12 +10478,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K40:BN40">
-    <cfRule type="expression" dxfId="56" priority="160">
+    <cfRule type="expression" dxfId="62" priority="164">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H63">
-    <cfRule type="dataBar" priority="139">
+  <conditionalFormatting sqref="H64">
+    <cfRule type="dataBar" priority="143">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10324,13 +10496,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K55:BN55">
-    <cfRule type="expression" dxfId="55" priority="148">
+  <conditionalFormatting sqref="K56:BN56">
+    <cfRule type="expression" dxfId="61" priority="152">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59">
-    <cfRule type="dataBar" priority="131">
+  <conditionalFormatting sqref="H60">
+    <cfRule type="dataBar" priority="135">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10343,13 +10515,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K63:BN63">
-    <cfRule type="expression" dxfId="54" priority="140">
+  <conditionalFormatting sqref="K64:BN64">
+    <cfRule type="expression" dxfId="60" priority="144">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H54">
-    <cfRule type="dataBar" priority="151">
+  <conditionalFormatting sqref="H55">
+    <cfRule type="dataBar" priority="155">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10362,13 +10534,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K54:BN54">
-    <cfRule type="expression" dxfId="53" priority="152">
+  <conditionalFormatting sqref="K55:BN55">
+    <cfRule type="expression" dxfId="59" priority="156">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H57">
-    <cfRule type="dataBar" priority="123">
+  <conditionalFormatting sqref="H58">
+    <cfRule type="dataBar" priority="127">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10381,13 +10553,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K59:BN59">
-    <cfRule type="expression" dxfId="52" priority="132">
+  <conditionalFormatting sqref="K60:BN60">
+    <cfRule type="expression" dxfId="58" priority="136">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H62">
-    <cfRule type="dataBar" priority="143">
+  <conditionalFormatting sqref="H63">
+    <cfRule type="dataBar" priority="147">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10400,13 +10572,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K62:BN62">
-    <cfRule type="expression" dxfId="51" priority="144">
+  <conditionalFormatting sqref="K63:BN63">
+    <cfRule type="expression" dxfId="57" priority="148">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="dataBar" priority="115">
+    <cfRule type="dataBar" priority="119">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10419,13 +10591,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K57:BN57">
-    <cfRule type="expression" dxfId="50" priority="124">
+  <conditionalFormatting sqref="K58:BN58">
+    <cfRule type="expression" dxfId="56" priority="128">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H58">
-    <cfRule type="dataBar" priority="135">
+  <conditionalFormatting sqref="H59">
+    <cfRule type="dataBar" priority="139">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10438,13 +10610,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K58:BN58">
-    <cfRule type="expression" dxfId="49" priority="136">
+  <conditionalFormatting sqref="K59:BN59">
+    <cfRule type="expression" dxfId="55" priority="140">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="dataBar" priority="107">
+    <cfRule type="dataBar" priority="111">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10458,12 +10630,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K46:BN46">
-    <cfRule type="expression" dxfId="48" priority="116">
+    <cfRule type="expression" dxfId="54" priority="120">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H56">
-    <cfRule type="dataBar" priority="127">
+  <conditionalFormatting sqref="H57">
+    <cfRule type="dataBar" priority="131">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10476,13 +10648,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K56:BN56">
-    <cfRule type="expression" dxfId="47" priority="128">
+  <conditionalFormatting sqref="K57:BN57">
+    <cfRule type="expression" dxfId="53" priority="132">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H61">
-    <cfRule type="dataBar" priority="99">
+  <conditionalFormatting sqref="H62">
+    <cfRule type="dataBar" priority="103">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10496,12 +10668,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:BN44">
-    <cfRule type="expression" dxfId="46" priority="108">
+    <cfRule type="expression" dxfId="52" priority="112">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="dataBar" priority="119">
+    <cfRule type="dataBar" priority="123">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10515,12 +10687,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:BN45">
-    <cfRule type="expression" dxfId="45" priority="120">
+    <cfRule type="expression" dxfId="51" priority="124">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H29">
-    <cfRule type="dataBar" priority="95">
+    <cfRule type="dataBar" priority="99">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10533,13 +10705,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K61:BN61">
-    <cfRule type="expression" dxfId="44" priority="100">
+  <conditionalFormatting sqref="K62:BN62">
+    <cfRule type="expression" dxfId="50" priority="104">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H42">
-    <cfRule type="dataBar" priority="111">
+    <cfRule type="dataBar" priority="115">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10553,17 +10725,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K42:BN42">
-    <cfRule type="expression" dxfId="43" priority="112">
+    <cfRule type="expression" dxfId="49" priority="116">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K29:BN29">
-    <cfRule type="expression" dxfId="42" priority="96">
+    <cfRule type="expression" dxfId="48" priority="100">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H60">
-    <cfRule type="dataBar" priority="103">
+  <conditionalFormatting sqref="H61">
+    <cfRule type="dataBar" priority="107">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10576,13 +10748,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K60:BN60">
-    <cfRule type="expression" dxfId="41" priority="104">
+  <conditionalFormatting sqref="K61:BN61">
+    <cfRule type="expression" dxfId="47" priority="108">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H12">
-    <cfRule type="dataBar" priority="77">
+    <cfRule type="dataBar" priority="81">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10596,20 +10768,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="40" priority="79">
+    <cfRule type="expression" dxfId="46" priority="83">
       <formula>AND($E12&lt;=K$6,ROUNDDOWN(($F12-$E12+1)*$H12,0)+$E12-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="80">
+    <cfRule type="expression" dxfId="45" priority="84">
       <formula>AND(NOT(ISBLANK($E12)),$E12&lt;=K$6,$F12&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:BN12">
-    <cfRule type="expression" dxfId="38" priority="78">
+    <cfRule type="expression" dxfId="44" priority="82">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H19">
-    <cfRule type="dataBar" priority="73">
+    <cfRule type="dataBar" priority="77">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10623,20 +10795,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="37" priority="75">
+    <cfRule type="expression" dxfId="43" priority="79">
       <formula>AND($E19&lt;=K$6,ROUNDDOWN(($F19-$E19+1)*$H19,0)+$E19-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="76">
+    <cfRule type="expression" dxfId="42" priority="80">
       <formula>AND(NOT(ISBLANK($E19)),$E19&lt;=K$6,$F19&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K19:BN19">
-    <cfRule type="expression" dxfId="35" priority="74">
+    <cfRule type="expression" dxfId="41" priority="78">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="dataBar" priority="69">
+    <cfRule type="dataBar" priority="73">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10650,20 +10822,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN31">
-    <cfRule type="expression" dxfId="34" priority="71">
+    <cfRule type="expression" dxfId="40" priority="75">
       <formula>AND($E31&lt;=K$6,ROUNDDOWN(($F31-$E31+1)*$H31,0)+$E31-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="72">
+    <cfRule type="expression" dxfId="39" priority="76">
       <formula>AND(NOT(ISBLANK($E31)),$E31&lt;=K$6,$F31&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:BN31">
-    <cfRule type="expression" dxfId="32" priority="70">
+    <cfRule type="expression" dxfId="38" priority="74">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="dataBar" priority="65">
+    <cfRule type="dataBar" priority="69">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10677,12 +10849,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K43:BN43">
-    <cfRule type="expression" dxfId="31" priority="66">
+    <cfRule type="expression" dxfId="37" priority="70">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="dataBar" priority="63">
+    <cfRule type="dataBar" priority="67">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10696,12 +10868,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K45:BN45">
-    <cfRule type="expression" dxfId="30" priority="64">
+    <cfRule type="expression" dxfId="36" priority="68">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="dataBar" priority="59">
+    <cfRule type="dataBar" priority="63">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10715,12 +10887,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K44:BN44">
-    <cfRule type="expression" dxfId="29" priority="60">
+    <cfRule type="expression" dxfId="35" priority="64">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H50">
-    <cfRule type="dataBar" priority="53">
+    <cfRule type="dataBar" priority="57">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10734,7 +10906,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="dataBar" priority="51">
+    <cfRule type="dataBar" priority="55">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10748,17 +10920,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K50:BN50">
-    <cfRule type="expression" dxfId="28" priority="54">
+    <cfRule type="expression" dxfId="34" priority="58">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:BN48">
-    <cfRule type="expression" dxfId="27" priority="52">
+    <cfRule type="expression" dxfId="33" priority="56">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="dataBar" priority="55">
+    <cfRule type="dataBar" priority="59">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10772,12 +10944,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:BN49">
-    <cfRule type="expression" dxfId="26" priority="56">
+    <cfRule type="expression" dxfId="32" priority="60">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H47">
-    <cfRule type="dataBar" priority="47">
+    <cfRule type="dataBar" priority="51">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10791,12 +10963,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K47:BN47">
-    <cfRule type="expression" dxfId="25" priority="48">
+    <cfRule type="expression" dxfId="31" priority="52">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="dataBar" priority="45">
+    <cfRule type="dataBar" priority="49">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10810,12 +10982,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K49:BN49">
-    <cfRule type="expression" dxfId="24" priority="46">
+    <cfRule type="expression" dxfId="30" priority="50">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H48">
-    <cfRule type="dataBar" priority="41">
+    <cfRule type="dataBar" priority="45">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10829,12 +11001,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K48:BN48">
-    <cfRule type="expression" dxfId="23" priority="42">
+    <cfRule type="expression" dxfId="29" priority="46">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="dataBar" priority="35">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10848,12 +11020,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:BN52">
-    <cfRule type="expression" dxfId="22" priority="36">
+    <cfRule type="expression" dxfId="28" priority="40">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="dataBar" priority="37">
+    <cfRule type="dataBar" priority="41">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10867,12 +11039,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:BN53">
-    <cfRule type="expression" dxfId="21" priority="38">
+    <cfRule type="expression" dxfId="27" priority="42">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="dataBar" priority="31">
+    <cfRule type="dataBar" priority="35">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10886,12 +11058,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K51:BN51">
-    <cfRule type="expression" dxfId="20" priority="32">
+    <cfRule type="expression" dxfId="26" priority="36">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H53">
-    <cfRule type="dataBar" priority="29">
+    <cfRule type="dataBar" priority="33">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10905,12 +11077,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K53:BN53">
-    <cfRule type="expression" dxfId="19" priority="30">
+    <cfRule type="expression" dxfId="25" priority="34">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52">
-    <cfRule type="dataBar" priority="25">
+    <cfRule type="dataBar" priority="29">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10924,12 +11096,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K52:BN52">
-    <cfRule type="expression" dxfId="18" priority="26">
+    <cfRule type="expression" dxfId="24" priority="30">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H32">
-    <cfRule type="dataBar" priority="21">
+    <cfRule type="dataBar" priority="25">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10943,28 +11115,28 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN32">
-    <cfRule type="expression" dxfId="17" priority="23">
+    <cfRule type="expression" dxfId="23" priority="27">
       <formula>AND($E32&lt;=K$6,ROUNDDOWN(($F32-$E32+1)*$H32,0)+$E32-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="16" priority="24">
+    <cfRule type="expression" dxfId="22" priority="28">
       <formula>AND(NOT(ISBLANK($E32)),$E32&lt;=K$6,$F32&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K32:BN32">
-    <cfRule type="expression" dxfId="15" priority="22">
+    <cfRule type="expression" dxfId="21" priority="26">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:BN35">
-    <cfRule type="expression" dxfId="14" priority="19">
+    <cfRule type="expression" dxfId="20" priority="23">
       <formula>AND($E35&lt;=K$6,ROUNDDOWN(($F35-$E35+1)*$H35,0)+$E35-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="19" priority="24">
       <formula>AND(NOT(ISBLANK($E35)),$E35&lt;=K$6,$F35&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H35">
-    <cfRule type="dataBar" priority="17">
+    <cfRule type="dataBar" priority="21">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -10978,20 +11150,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K35:BN35">
-    <cfRule type="expression" dxfId="12" priority="18">
+    <cfRule type="expression" dxfId="18" priority="22">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN36">
-    <cfRule type="expression" dxfId="11" priority="15">
+    <cfRule type="expression" dxfId="17" priority="19">
       <formula>AND($E36&lt;=K$6,ROUNDDOWN(($F36-$E36+1)*$H36,0)+$E36-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="16">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>AND(NOT(ISBLANK($E36)),$E36&lt;=K$6,$F36&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36">
-    <cfRule type="dataBar" priority="13">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11005,20 +11177,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K36:BN36">
-    <cfRule type="expression" dxfId="9" priority="14">
+    <cfRule type="expression" dxfId="15" priority="18">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:BN37">
-    <cfRule type="expression" dxfId="8" priority="11">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>AND($E37&lt;=K$6,ROUNDDOWN(($F37-$E37+1)*$H37,0)+$E37-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="12">
+    <cfRule type="expression" dxfId="13" priority="16">
       <formula>AND(NOT(ISBLANK($E37)),$E37&lt;=K$6,$F37&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H37">
-    <cfRule type="dataBar" priority="9">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11032,20 +11204,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K37:BN37">
-    <cfRule type="expression" dxfId="6" priority="10">
+    <cfRule type="expression" dxfId="12" priority="14">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:BN38">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="11" priority="11">
       <formula>AND($E38&lt;=K$6,ROUNDDOWN(($F38-$E38+1)*$H38,0)+$E38-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="10" priority="12">
       <formula>AND(NOT(ISBLANK($E38)),$E38&lt;=K$6,$F38&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38">
-    <cfRule type="dataBar" priority="5">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11059,20 +11231,20 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K38:BN38">
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:BN39">
-    <cfRule type="expression" dxfId="2" priority="3">
+    <cfRule type="expression" dxfId="8" priority="7">
       <formula>AND($E39&lt;=K$6,ROUNDDOWN(($F39-$E39+1)*$H39,0)+$E39-1&gt;=K$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>AND(NOT(ISBLANK($E39)),$E39&lt;=K$6,$F39&gt;=K$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H39">
-    <cfRule type="dataBar" priority="1">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -11086,18 +11258,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K39:BN39">
+    <cfRule type="expression" dxfId="6" priority="6">
+      <formula>K$6=TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0" tint="-0.34998626667073579"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{DEC8A02F-80BB-FF4A-8656-257DA44E514E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K54:BN54">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>AND($E54&lt;=K$6,ROUNDDOWN(($F54-$E54+1)*$H54,0)+$E54-1&gt;=K$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="4">
+      <formula>AND(NOT(ISBLANK($E54)),$E54&lt;=K$6,$F54&gt;=K$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K54:BN54">
     <cfRule type="expression" dxfId="0" priority="2">
       <formula>K$6=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation allowBlank="1" showInputMessage="1" promptTitle="Display Week" prompt="Enter the week number to display first in the Gantt Chart. The weeks are numbered starting from the week containing the Project Start Date." sqref="H4"/>
   </dataValidations>
   <pageMargins left="0.25" right="0.25" top="0.5" bottom="0.5" header="0.5" footer="0.25"/>
   <pageSetup scale="63" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
   <ignoredErrors>
-    <ignoredError sqref="A64:B64 A66:B66 B65 E10 E20 E24 E64:H66 G10:H10 G20:H20 G24:H24 G67 G68:G69 G70 G25" unlockedFormula="1"/>
+    <ignoredError sqref="A65:B65 A67:B67 B66 E10 E20 E24 E65:H67 G10:H10 G20:H20 G24:H24 G68 G69:G70 G71 G25" unlockedFormula="1"/>
     <ignoredError sqref="A24 A20 A10 A16" formula="1"/>
   </ignoredErrors>
   <drawing r:id="rId2"/>
@@ -11148,7 +11347,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H8:H11 H16:H18 H64:H70 H30 H20:H28 H13</xm:sqref>
+          <xm:sqref>H8:H11 H16:H18 H65:H71 H30 H20:H28 H13</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{C1E55C9C-328E-7F42-B324-A31B3CE69B6E}">
@@ -11238,7 +11437,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H55</xm:sqref>
+          <xm:sqref>H56</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D0208E98-1C87-F945-B7BA-D5E81A01579A}">
@@ -11268,7 +11467,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H63</xm:sqref>
+          <xm:sqref>H64</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{F222E3D4-7513-264C-968B-0292F382CD5D}">
@@ -11283,7 +11482,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H59</xm:sqref>
+          <xm:sqref>H60</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{526828FD-A928-6E46-95F8-D74ACD1E339B}">
@@ -11298,7 +11497,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H54</xm:sqref>
+          <xm:sqref>H55</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{730B0F02-39AB-BD42-BB2A-405EFC6279DF}">
@@ -11313,7 +11512,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H57</xm:sqref>
+          <xm:sqref>H58</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1C2DB213-53A8-4946-B60A-C01681F15068}">
@@ -11328,7 +11527,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H62</xm:sqref>
+          <xm:sqref>H63</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{D8388F22-1F90-F24E-9C6B-625491BBF15E}">
@@ -11358,7 +11557,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H58</xm:sqref>
+          <xm:sqref>H59</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6CC7F112-D4C4-2647-8F58-25080F8D0653}">
@@ -11388,7 +11587,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H56</xm:sqref>
+          <xm:sqref>H57</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{A44EC134-680C-6943-A530-937463E3A665}">
@@ -11403,7 +11602,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H61</xm:sqref>
+          <xm:sqref>H62</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{6900B624-12B9-8C44-99D7-233CE13C7600}">
@@ -11463,7 +11662,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>H60</xm:sqref>
+          <xm:sqref>H61</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{B72F9582-8103-A840-9EC3-CEB5270C8B2A}">
@@ -11810,6 +12009,21 @@
           </x14:cfRule>
           <xm:sqref>H39</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{DEC8A02F-80BB-FF4A-8656-257DA44E514E}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>H54</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
updated gantt chart and minutes
</commit_message>
<xml_diff>
--- a/0b_forms/gantt_chart.xlsx
+++ b/0b_forms/gantt_chart.xlsx
@@ -2700,6 +2700,24 @@
     <xf numFmtId="0" fontId="40" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="43" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="58" fillId="0" borderId="0" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2707,27 +2725,9 @@
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="43" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="43" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="59" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3591,7 +3591,7 @@
         <xdr:cNvPr id="8236" name="Text Box 44" hidden="1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002C200000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C200000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3655,7 +3655,7 @@
                   <a14:compatExt spid="_x0000_s8238"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00002E200000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E200000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3705,7 +3705,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3789,7 +3789,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3844,7 +3844,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000005000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3899,7 +3899,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4227,8 +4227,8 @@
   <dimension ref="A1:BN73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="107" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="7" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H45" sqref="H45"/>
+      <pane ySplit="7" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -4256,27 +4256,27 @@
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
       <c r="I1" s="126"/>
-      <c r="K1" s="173"/>
-      <c r="L1" s="173"/>
-      <c r="M1" s="173"/>
-      <c r="N1" s="173"/>
-      <c r="O1" s="173"/>
-      <c r="P1" s="173"/>
-      <c r="Q1" s="173"/>
-      <c r="R1" s="173"/>
-      <c r="S1" s="173"/>
-      <c r="T1" s="173"/>
-      <c r="U1" s="173"/>
-      <c r="V1" s="173"/>
-      <c r="W1" s="173"/>
-      <c r="X1" s="173"/>
-      <c r="Y1" s="173"/>
-      <c r="Z1" s="173"/>
-      <c r="AA1" s="173"/>
-      <c r="AB1" s="173"/>
-      <c r="AC1" s="173"/>
-      <c r="AD1" s="173"/>
-      <c r="AE1" s="173"/>
+      <c r="K1" s="179"/>
+      <c r="L1" s="179"/>
+      <c r="M1" s="179"/>
+      <c r="N1" s="179"/>
+      <c r="O1" s="179"/>
+      <c r="P1" s="179"/>
+      <c r="Q1" s="179"/>
+      <c r="R1" s="179"/>
+      <c r="S1" s="179"/>
+      <c r="T1" s="179"/>
+      <c r="U1" s="179"/>
+      <c r="V1" s="179"/>
+      <c r="W1" s="179"/>
+      <c r="X1" s="179"/>
+      <c r="Y1" s="179"/>
+      <c r="Z1" s="179"/>
+      <c r="AA1" s="179"/>
+      <c r="AB1" s="179"/>
+      <c r="AC1" s="179"/>
+      <c r="AD1" s="179"/>
+      <c r="AE1" s="179"/>
     </row>
     <row r="2" spans="1:66" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="52" t="s">
@@ -4321,11 +4321,11 @@
       <c r="B4" s="111" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="178">
+      <c r="C4" s="181">
         <v>43374</v>
       </c>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
       <c r="F4" s="108"/>
       <c r="G4" s="111" t="s">
         <v>73</v>
@@ -4335,182 +4335,182 @@
       </c>
       <c r="I4" s="109"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="175" t="str">
+      <c r="K4" s="173" t="str">
         <f>"Week "&amp;(K6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 4</v>
       </c>
-      <c r="L4" s="176"/>
-      <c r="M4" s="176"/>
-      <c r="N4" s="176"/>
-      <c r="O4" s="176"/>
-      <c r="P4" s="176"/>
-      <c r="Q4" s="177"/>
-      <c r="R4" s="175" t="str">
+      <c r="L4" s="174"/>
+      <c r="M4" s="174"/>
+      <c r="N4" s="174"/>
+      <c r="O4" s="174"/>
+      <c r="P4" s="174"/>
+      <c r="Q4" s="175"/>
+      <c r="R4" s="173" t="str">
         <f>"Week "&amp;(R6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 5</v>
       </c>
-      <c r="S4" s="176"/>
-      <c r="T4" s="176"/>
-      <c r="U4" s="176"/>
-      <c r="V4" s="176"/>
-      <c r="W4" s="176"/>
-      <c r="X4" s="177"/>
-      <c r="Y4" s="175" t="str">
+      <c r="S4" s="174"/>
+      <c r="T4" s="174"/>
+      <c r="U4" s="174"/>
+      <c r="V4" s="174"/>
+      <c r="W4" s="174"/>
+      <c r="X4" s="175"/>
+      <c r="Y4" s="173" t="str">
         <f>"Week "&amp;(Y6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 6</v>
       </c>
-      <c r="Z4" s="176"/>
-      <c r="AA4" s="176"/>
-      <c r="AB4" s="176"/>
-      <c r="AC4" s="176"/>
-      <c r="AD4" s="176"/>
-      <c r="AE4" s="177"/>
-      <c r="AF4" s="175" t="str">
+      <c r="Z4" s="174"/>
+      <c r="AA4" s="174"/>
+      <c r="AB4" s="174"/>
+      <c r="AC4" s="174"/>
+      <c r="AD4" s="174"/>
+      <c r="AE4" s="175"/>
+      <c r="AF4" s="173" t="str">
         <f>"Week "&amp;(AF6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 7</v>
       </c>
-      <c r="AG4" s="176"/>
-      <c r="AH4" s="176"/>
-      <c r="AI4" s="176"/>
-      <c r="AJ4" s="176"/>
-      <c r="AK4" s="176"/>
-      <c r="AL4" s="177"/>
-      <c r="AM4" s="175" t="str">
+      <c r="AG4" s="174"/>
+      <c r="AH4" s="174"/>
+      <c r="AI4" s="174"/>
+      <c r="AJ4" s="174"/>
+      <c r="AK4" s="174"/>
+      <c r="AL4" s="175"/>
+      <c r="AM4" s="173" t="str">
         <f>"Week "&amp;(AM6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 8</v>
       </c>
-      <c r="AN4" s="176"/>
-      <c r="AO4" s="176"/>
-      <c r="AP4" s="176"/>
-      <c r="AQ4" s="176"/>
-      <c r="AR4" s="176"/>
-      <c r="AS4" s="177"/>
-      <c r="AT4" s="175" t="str">
+      <c r="AN4" s="174"/>
+      <c r="AO4" s="174"/>
+      <c r="AP4" s="174"/>
+      <c r="AQ4" s="174"/>
+      <c r="AR4" s="174"/>
+      <c r="AS4" s="175"/>
+      <c r="AT4" s="173" t="str">
         <f>"Week "&amp;(AT6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 9</v>
       </c>
-      <c r="AU4" s="176"/>
-      <c r="AV4" s="176"/>
-      <c r="AW4" s="176"/>
-      <c r="AX4" s="176"/>
-      <c r="AY4" s="176"/>
-      <c r="AZ4" s="177"/>
-      <c r="BA4" s="175" t="str">
+      <c r="AU4" s="174"/>
+      <c r="AV4" s="174"/>
+      <c r="AW4" s="174"/>
+      <c r="AX4" s="174"/>
+      <c r="AY4" s="174"/>
+      <c r="AZ4" s="175"/>
+      <c r="BA4" s="173" t="str">
         <f>"Week "&amp;(BA6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 10</v>
       </c>
-      <c r="BB4" s="176"/>
-      <c r="BC4" s="176"/>
-      <c r="BD4" s="176"/>
-      <c r="BE4" s="176"/>
-      <c r="BF4" s="176"/>
-      <c r="BG4" s="177"/>
-      <c r="BH4" s="175" t="str">
+      <c r="BB4" s="174"/>
+      <c r="BC4" s="174"/>
+      <c r="BD4" s="174"/>
+      <c r="BE4" s="174"/>
+      <c r="BF4" s="174"/>
+      <c r="BG4" s="175"/>
+      <c r="BH4" s="173" t="str">
         <f>"Week "&amp;(BH6-($C$4-WEEKDAY($C$4,1)+2))/7+1</f>
         <v>Week 11</v>
       </c>
-      <c r="BI4" s="176"/>
-      <c r="BJ4" s="176"/>
-      <c r="BK4" s="176"/>
-      <c r="BL4" s="176"/>
-      <c r="BM4" s="176"/>
-      <c r="BN4" s="177"/>
+      <c r="BI4" s="174"/>
+      <c r="BJ4" s="174"/>
+      <c r="BK4" s="174"/>
+      <c r="BL4" s="174"/>
+      <c r="BM4" s="174"/>
+      <c r="BN4" s="175"/>
     </row>
     <row r="5" spans="1:66" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="107"/>
       <c r="B5" s="111" t="s">
         <v>75</v>
       </c>
-      <c r="C5" s="174">
+      <c r="C5" s="180">
         <v>43612</v>
       </c>
-      <c r="D5" s="174"/>
-      <c r="E5" s="174"/>
+      <c r="D5" s="180"/>
+      <c r="E5" s="180"/>
       <c r="F5" s="110"/>
       <c r="G5" s="110"/>
       <c r="H5" s="110"/>
       <c r="I5" s="110"/>
       <c r="J5" s="50"/>
-      <c r="K5" s="179">
+      <c r="K5" s="176">
         <f>K6</f>
         <v>43395</v>
       </c>
-      <c r="L5" s="180"/>
-      <c r="M5" s="180"/>
-      <c r="N5" s="180"/>
-      <c r="O5" s="180"/>
-      <c r="P5" s="180"/>
-      <c r="Q5" s="181"/>
-      <c r="R5" s="179">
+      <c r="L5" s="177"/>
+      <c r="M5" s="177"/>
+      <c r="N5" s="177"/>
+      <c r="O5" s="177"/>
+      <c r="P5" s="177"/>
+      <c r="Q5" s="178"/>
+      <c r="R5" s="176">
         <f>R6</f>
         <v>43402</v>
       </c>
-      <c r="S5" s="180"/>
-      <c r="T5" s="180"/>
-      <c r="U5" s="180"/>
-      <c r="V5" s="180"/>
-      <c r="W5" s="180"/>
-      <c r="X5" s="181"/>
-      <c r="Y5" s="179">
+      <c r="S5" s="177"/>
+      <c r="T5" s="177"/>
+      <c r="U5" s="177"/>
+      <c r="V5" s="177"/>
+      <c r="W5" s="177"/>
+      <c r="X5" s="178"/>
+      <c r="Y5" s="176">
         <f>Y6</f>
         <v>43409</v>
       </c>
-      <c r="Z5" s="180"/>
-      <c r="AA5" s="180"/>
-      <c r="AB5" s="180"/>
-      <c r="AC5" s="180"/>
-      <c r="AD5" s="180"/>
-      <c r="AE5" s="181"/>
-      <c r="AF5" s="179">
+      <c r="Z5" s="177"/>
+      <c r="AA5" s="177"/>
+      <c r="AB5" s="177"/>
+      <c r="AC5" s="177"/>
+      <c r="AD5" s="177"/>
+      <c r="AE5" s="178"/>
+      <c r="AF5" s="176">
         <f>AF6</f>
         <v>43416</v>
       </c>
-      <c r="AG5" s="180"/>
-      <c r="AH5" s="180"/>
-      <c r="AI5" s="180"/>
-      <c r="AJ5" s="180"/>
-      <c r="AK5" s="180"/>
-      <c r="AL5" s="181"/>
-      <c r="AM5" s="179">
+      <c r="AG5" s="177"/>
+      <c r="AH5" s="177"/>
+      <c r="AI5" s="177"/>
+      <c r="AJ5" s="177"/>
+      <c r="AK5" s="177"/>
+      <c r="AL5" s="178"/>
+      <c r="AM5" s="176">
         <f>AM6</f>
         <v>43423</v>
       </c>
-      <c r="AN5" s="180"/>
-      <c r="AO5" s="180"/>
-      <c r="AP5" s="180"/>
-      <c r="AQ5" s="180"/>
-      <c r="AR5" s="180"/>
-      <c r="AS5" s="181"/>
-      <c r="AT5" s="179">
+      <c r="AN5" s="177"/>
+      <c r="AO5" s="177"/>
+      <c r="AP5" s="177"/>
+      <c r="AQ5" s="177"/>
+      <c r="AR5" s="177"/>
+      <c r="AS5" s="178"/>
+      <c r="AT5" s="176">
         <f>AT6</f>
         <v>43430</v>
       </c>
-      <c r="AU5" s="180"/>
-      <c r="AV5" s="180"/>
-      <c r="AW5" s="180"/>
-      <c r="AX5" s="180"/>
-      <c r="AY5" s="180"/>
-      <c r="AZ5" s="181"/>
-      <c r="BA5" s="179">
+      <c r="AU5" s="177"/>
+      <c r="AV5" s="177"/>
+      <c r="AW5" s="177"/>
+      <c r="AX5" s="177"/>
+      <c r="AY5" s="177"/>
+      <c r="AZ5" s="178"/>
+      <c r="BA5" s="176">
         <f>BA6</f>
         <v>43437</v>
       </c>
-      <c r="BB5" s="180"/>
-      <c r="BC5" s="180"/>
-      <c r="BD5" s="180"/>
-      <c r="BE5" s="180"/>
-      <c r="BF5" s="180"/>
-      <c r="BG5" s="181"/>
-      <c r="BH5" s="179">
+      <c r="BB5" s="177"/>
+      <c r="BC5" s="177"/>
+      <c r="BD5" s="177"/>
+      <c r="BE5" s="177"/>
+      <c r="BF5" s="177"/>
+      <c r="BG5" s="178"/>
+      <c r="BH5" s="176">
         <f>BH6</f>
         <v>43444</v>
       </c>
-      <c r="BI5" s="180"/>
-      <c r="BJ5" s="180"/>
-      <c r="BK5" s="180"/>
-      <c r="BL5" s="180"/>
-      <c r="BM5" s="180"/>
-      <c r="BN5" s="181"/>
+      <c r="BI5" s="177"/>
+      <c r="BJ5" s="177"/>
+      <c r="BK5" s="177"/>
+      <c r="BL5" s="177"/>
+      <c r="BM5" s="177"/>
+      <c r="BN5" s="178"/>
     </row>
     <row r="6" spans="1:66" x14ac:dyDescent="0.15">
       <c r="A6" s="49"/>
@@ -8445,7 +8445,7 @@
         <v>6</v>
       </c>
       <c r="H49" s="63">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="I49" s="80">
         <f>IF(OR(F49=0,E49=0)," - ",NETWORKDAYS(E49,F49))</f>
@@ -8614,7 +8614,9 @@
       <c r="G51" s="62">
         <v>6</v>
       </c>
-      <c r="H51" s="63"/>
+      <c r="H51" s="63">
+        <v>1</v>
+      </c>
       <c r="I51" s="80">
         <f t="shared" si="31"/>
         <v>5</v>
@@ -8944,7 +8946,9 @@
       <c r="G55" s="62">
         <v>7</v>
       </c>
-      <c r="H55" s="63"/>
+      <c r="H55" s="63">
+        <v>1</v>
+      </c>
       <c r="I55" s="80">
         <f t="shared" ref="I55" si="33">IF(OR(F55=0,E55=0)," - ",NETWORKDAYS(E55,F55))</f>
         <v>5</v>
@@ -10380,6 +10384,15 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertRows="0" deleteRows="0"/>
   <mergeCells count="19">
+    <mergeCell ref="K1:AE1"/>
+    <mergeCell ref="C5:E5"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="R5:X5"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="Y4:AE4"/>
+    <mergeCell ref="Y5:AE5"/>
     <mergeCell ref="AF4:AL4"/>
     <mergeCell ref="AF5:AL5"/>
     <mergeCell ref="BH4:BN4"/>
@@ -10390,15 +10403,6 @@
     <mergeCell ref="AM4:AS4"/>
     <mergeCell ref="BA4:BG4"/>
     <mergeCell ref="BA5:BG5"/>
-    <mergeCell ref="K1:AE1"/>
-    <mergeCell ref="C5:E5"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="K4:Q4"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="R5:X5"/>
-    <mergeCell ref="K5:Q5"/>
-    <mergeCell ref="Y4:AE4"/>
-    <mergeCell ref="Y5:AE5"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="H8:H11 H16:H18 H66:H72 H30 H20:H28 H13">

</xml_diff>